<commit_message>
Reset môi trường code
</commit_message>
<xml_diff>
--- a/Essay/Nhom6_KinhDoanhRuou_OPPM.xlsx
+++ b/Essay/Nhom6_KinhDoanhRuou_OPPM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuan Hung\Desktop\Learning\Exercise\SGU Software Technology - Mr Canh\Software-Technology-Project\Essay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology-Project\Essay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0BC49F-B9C1-4F88-AA49-52B1EB29E7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577004DE-0AB0-4470-AB63-851C5168D06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Charter" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0&quot;M&quot;;_(&quot;$&quot;* \(#,##0.0&quot;M&quot;\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0000"/>
     <numFmt numFmtId="167" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="169" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="53" x14ac:knownFonts="1">
     <font>
@@ -2922,12 +2922,454 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2940,27 +3382,9 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2970,21 +3394,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2994,16 +3403,16 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="40" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="40" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="40" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="40" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="40" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3015,372 +3424,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3390,6 +3433,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="74" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="78" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -3402,24 +3456,228 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="115" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="116" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="117" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="115" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="116" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="117" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="113" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="114" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="78" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="40" fillId="0" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="73" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="80" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="82" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="5" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="86" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="89" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="94" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="87" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="90" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="95" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="88" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="91" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="96" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="37" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="4" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="4" borderId="77" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -3440,278 +3698,20 @@
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="86" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="89" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="94" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="87" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="90" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="95" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="88" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="91" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="96" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="37" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="82" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="113" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="114" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="115" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="116" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="117" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="4" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="74" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="75" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="4" borderId="77" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="78" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="79" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="40" fillId="0" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="74" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="75" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="73" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="80" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="78" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="79" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="115" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="116" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="117" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="4" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4230,15 +4230,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>89535</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>74295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>194310</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>115430</xdr:rowOff>
+      <xdr:rowOff>123050</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4255,7 +4255,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="340995" y="241935"/>
+          <a:off x="325755" y="249555"/>
           <a:ext cx="714375" cy="726935"/>
           <a:chOff x="-9144" y="4390225"/>
           <a:chExt cx="2249424" cy="2376335"/>
@@ -4864,774 +4864,774 @@
   <sheetData>
     <row r="1" spans="2:13" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="295" t="s">
+      <c r="B2" s="188" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="296"/>
-      <c r="D2" s="296"/>
-      <c r="E2" s="296"/>
-      <c r="F2" s="296"/>
-      <c r="G2" s="296"/>
-      <c r="H2" s="296"/>
-      <c r="I2" s="296"/>
-      <c r="J2" s="296"/>
-      <c r="K2" s="296"/>
-      <c r="L2" s="296"/>
-      <c r="M2" s="297"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
+      <c r="L2" s="189"/>
+      <c r="M2" s="190"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="298"/>
-      <c r="C3" s="299"/>
-      <c r="D3" s="299"/>
-      <c r="E3" s="299"/>
-      <c r="F3" s="299"/>
-      <c r="G3" s="299"/>
-      <c r="H3" s="299"/>
-      <c r="I3" s="299"/>
-      <c r="J3" s="299"/>
-      <c r="K3" s="299"/>
-      <c r="L3" s="299"/>
-      <c r="M3" s="300"/>
+      <c r="B3" s="191"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="192"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="193"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="153"/>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="316" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
-      <c r="K4" s="171"/>
-      <c r="L4" s="171"/>
-      <c r="M4" s="172"/>
+      <c r="D4" s="316"/>
+      <c r="E4" s="316"/>
+      <c r="F4" s="316"/>
+      <c r="G4" s="316"/>
+      <c r="H4" s="316"/>
+      <c r="I4" s="316"/>
+      <c r="J4" s="316"/>
+      <c r="K4" s="316"/>
+      <c r="L4" s="316"/>
+      <c r="M4" s="317"/>
     </row>
     <row r="5" spans="2:13" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="319"/>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
-      <c r="G5" s="320"/>
-      <c r="H5" s="320"/>
-      <c r="I5" s="320"/>
-      <c r="J5" s="320"/>
-      <c r="K5" s="320"/>
-      <c r="L5" s="320"/>
-      <c r="M5" s="321"/>
+      <c r="B5" s="215"/>
+      <c r="C5" s="216"/>
+      <c r="D5" s="216"/>
+      <c r="E5" s="216"/>
+      <c r="F5" s="216"/>
+      <c r="G5" s="216"/>
+      <c r="H5" s="216"/>
+      <c r="I5" s="216"/>
+      <c r="J5" s="216"/>
+      <c r="K5" s="216"/>
+      <c r="L5" s="216"/>
+      <c r="M5" s="217"/>
     </row>
     <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="307" t="s">
+      <c r="B6" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="308"/>
-      <c r="D6" s="309"/>
-      <c r="E6" s="309"/>
-      <c r="F6" s="310"/>
-      <c r="G6" s="310"/>
-      <c r="H6" s="310"/>
-      <c r="I6" s="310"/>
-      <c r="J6" s="310"/>
-      <c r="K6" s="310"/>
-      <c r="L6" s="310"/>
-      <c r="M6" s="311"/>
+      <c r="C6" s="201"/>
+      <c r="D6" s="202"/>
+      <c r="E6" s="202"/>
+      <c r="F6" s="203"/>
+      <c r="G6" s="203"/>
+      <c r="H6" s="203"/>
+      <c r="I6" s="203"/>
+      <c r="J6" s="203"/>
+      <c r="K6" s="203"/>
+      <c r="L6" s="203"/>
+      <c r="M6" s="204"/>
     </row>
     <row r="7" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="187" t="s">
+      <c r="B7" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="188"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
-      <c r="F7" s="312"/>
-      <c r="G7" s="312"/>
-      <c r="H7" s="312"/>
-      <c r="I7" s="312"/>
-      <c r="J7" s="312"/>
-      <c r="K7" s="312"/>
-      <c r="L7" s="312"/>
-      <c r="M7" s="313"/>
+      <c r="C7" s="206"/>
+      <c r="D7" s="207"/>
+      <c r="E7" s="207"/>
+      <c r="F7" s="208"/>
+      <c r="G7" s="208"/>
+      <c r="H7" s="208"/>
+      <c r="I7" s="208"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="208"/>
+      <c r="L7" s="208"/>
+      <c r="M7" s="209"/>
     </row>
     <row r="8" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="314" t="s">
+      <c r="B8" s="210" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="315"/>
-      <c r="D8" s="316"/>
-      <c r="E8" s="316"/>
-      <c r="F8" s="317"/>
-      <c r="G8" s="317"/>
-      <c r="H8" s="317"/>
-      <c r="I8" s="317"/>
-      <c r="J8" s="317"/>
-      <c r="K8" s="317"/>
-      <c r="L8" s="317"/>
-      <c r="M8" s="318"/>
+      <c r="C8" s="211"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="213"/>
+      <c r="G8" s="213"/>
+      <c r="H8" s="213"/>
+      <c r="I8" s="213"/>
+      <c r="J8" s="213"/>
+      <c r="K8" s="213"/>
+      <c r="L8" s="213"/>
+      <c r="M8" s="214"/>
     </row>
     <row r="9" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="187" t="s">
+      <c r="B9" s="205" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="188"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="312"/>
-      <c r="G9" s="312"/>
-      <c r="H9" s="312"/>
-      <c r="I9" s="312"/>
-      <c r="J9" s="312"/>
-      <c r="K9" s="312"/>
-      <c r="L9" s="312"/>
-      <c r="M9" s="313"/>
+      <c r="C9" s="206"/>
+      <c r="D9" s="207"/>
+      <c r="E9" s="207"/>
+      <c r="F9" s="208"/>
+      <c r="G9" s="208"/>
+      <c r="H9" s="208"/>
+      <c r="I9" s="208"/>
+      <c r="J9" s="208"/>
+      <c r="K9" s="208"/>
+      <c r="L9" s="208"/>
+      <c r="M9" s="209"/>
     </row>
     <row r="10" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="314" t="s">
+      <c r="B10" s="210" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="315"/>
-      <c r="D10" s="316"/>
-      <c r="E10" s="316"/>
-      <c r="F10" s="317"/>
-      <c r="G10" s="317"/>
-      <c r="H10" s="317"/>
-      <c r="I10" s="317"/>
-      <c r="J10" s="317"/>
-      <c r="K10" s="317"/>
-      <c r="L10" s="317"/>
-      <c r="M10" s="318"/>
+      <c r="C10" s="211"/>
+      <c r="D10" s="212"/>
+      <c r="E10" s="212"/>
+      <c r="F10" s="213"/>
+      <c r="G10" s="213"/>
+      <c r="H10" s="213"/>
+      <c r="I10" s="213"/>
+      <c r="J10" s="213"/>
+      <c r="K10" s="213"/>
+      <c r="L10" s="213"/>
+      <c r="M10" s="214"/>
     </row>
     <row r="11" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="187" t="s">
+      <c r="B11" s="205" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="189"/>
-      <c r="E11" s="189"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="193"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="194"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="327"/>
+      <c r="G11" s="327"/>
+      <c r="H11" s="327"/>
+      <c r="I11" s="327"/>
+      <c r="J11" s="327"/>
+      <c r="K11" s="327"/>
+      <c r="L11" s="327"/>
+      <c r="M11" s="328"/>
     </row>
     <row r="12" spans="2:13" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="190" t="s">
+      <c r="B12" s="324" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="191"/>
-      <c r="D12" s="192"/>
-      <c r="E12" s="192"/>
-      <c r="F12" s="195"/>
-      <c r="G12" s="195"/>
-      <c r="H12" s="195"/>
-      <c r="I12" s="195"/>
-      <c r="J12" s="195"/>
-      <c r="K12" s="195"/>
-      <c r="L12" s="195"/>
-      <c r="M12" s="196"/>
+      <c r="C12" s="325"/>
+      <c r="D12" s="326"/>
+      <c r="E12" s="326"/>
+      <c r="F12" s="329"/>
+      <c r="G12" s="329"/>
+      <c r="H12" s="329"/>
+      <c r="I12" s="329"/>
+      <c r="J12" s="329"/>
+      <c r="K12" s="329"/>
+      <c r="L12" s="329"/>
+      <c r="M12" s="330"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="179" t="s">
+      <c r="B13" s="248" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="180"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="180"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="180"/>
-      <c r="J13" s="180"/>
-      <c r="K13" s="180"/>
-      <c r="L13" s="180"/>
-      <c r="M13" s="181"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="249"/>
+      <c r="H13" s="249"/>
+      <c r="I13" s="249"/>
+      <c r="J13" s="249"/>
+      <c r="K13" s="249"/>
+      <c r="L13" s="249"/>
+      <c r="M13" s="250"/>
     </row>
     <row r="14" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="173" t="s">
+      <c r="B14" s="318" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="174"/>
-      <c r="D14" s="182" t="s">
+      <c r="C14" s="319"/>
+      <c r="D14" s="321" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="182"/>
-      <c r="F14" s="183"/>
-      <c r="G14" s="183"/>
-      <c r="H14" s="183"/>
-      <c r="I14" s="183"/>
-      <c r="J14" s="183"/>
-      <c r="K14" s="183"/>
-      <c r="L14" s="183"/>
-      <c r="M14" s="184"/>
+      <c r="E14" s="321"/>
+      <c r="F14" s="322"/>
+      <c r="G14" s="322"/>
+      <c r="H14" s="322"/>
+      <c r="I14" s="322"/>
+      <c r="J14" s="322"/>
+      <c r="K14" s="322"/>
+      <c r="L14" s="322"/>
+      <c r="M14" s="323"/>
     </row>
     <row r="15" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="175" t="s">
+      <c r="B15" s="292" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="176"/>
-      <c r="D15" s="249" t="s">
+      <c r="C15" s="254"/>
+      <c r="D15" s="244" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="249"/>
-      <c r="F15" s="185"/>
-      <c r="G15" s="185"/>
-      <c r="H15" s="185"/>
-      <c r="I15" s="185"/>
-      <c r="J15" s="185"/>
-      <c r="K15" s="185"/>
-      <c r="L15" s="185"/>
-      <c r="M15" s="186"/>
+      <c r="E15" s="244"/>
+      <c r="F15" s="183"/>
+      <c r="G15" s="183"/>
+      <c r="H15" s="183"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="183"/>
+      <c r="K15" s="183"/>
+      <c r="L15" s="183"/>
+      <c r="M15" s="184"/>
     </row>
     <row r="16" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="320" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="178"/>
-      <c r="D16" s="197" t="s">
+      <c r="C16" s="235"/>
+      <c r="D16" s="331" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="197"/>
-      <c r="F16" s="198"/>
-      <c r="G16" s="198"/>
-      <c r="H16" s="198"/>
-      <c r="I16" s="198"/>
-      <c r="J16" s="198"/>
-      <c r="K16" s="198"/>
-      <c r="L16" s="198"/>
-      <c r="M16" s="199"/>
+      <c r="E16" s="331"/>
+      <c r="F16" s="332"/>
+      <c r="G16" s="332"/>
+      <c r="H16" s="332"/>
+      <c r="I16" s="332"/>
+      <c r="J16" s="332"/>
+      <c r="K16" s="332"/>
+      <c r="L16" s="332"/>
+      <c r="M16" s="333"/>
     </row>
     <row r="17" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="175" t="s">
+      <c r="B17" s="292" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="176"/>
-      <c r="D17" s="200" t="s">
+      <c r="C17" s="254"/>
+      <c r="D17" s="218" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="200"/>
-      <c r="F17" s="185"/>
-      <c r="G17" s="185"/>
-      <c r="H17" s="185"/>
-      <c r="I17" s="185"/>
-      <c r="J17" s="185"/>
-      <c r="K17" s="185"/>
-      <c r="L17" s="185"/>
-      <c r="M17" s="186"/>
+      <c r="E17" s="218"/>
+      <c r="F17" s="183"/>
+      <c r="G17" s="183"/>
+      <c r="H17" s="183"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="183"/>
+      <c r="K17" s="183"/>
+      <c r="L17" s="183"/>
+      <c r="M17" s="184"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="286" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="241"/>
-      <c r="D18" s="231" t="s">
+      <c r="C18" s="287"/>
+      <c r="D18" s="280" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="232"/>
-      <c r="F18" s="237">
+      <c r="E18" s="281"/>
+      <c r="F18" s="185">
         <v>1</v>
       </c>
-      <c r="G18" s="238"/>
-      <c r="H18" s="238"/>
-      <c r="I18" s="238"/>
-      <c r="J18" s="238"/>
-      <c r="K18" s="238"/>
-      <c r="L18" s="238"/>
-      <c r="M18" s="239"/>
+      <c r="G18" s="186"/>
+      <c r="H18" s="186"/>
+      <c r="I18" s="186"/>
+      <c r="J18" s="186"/>
+      <c r="K18" s="186"/>
+      <c r="L18" s="186"/>
+      <c r="M18" s="187"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="242"/>
-      <c r="C19" s="243"/>
-      <c r="D19" s="233"/>
-      <c r="E19" s="234"/>
-      <c r="F19" s="237">
+      <c r="B19" s="288"/>
+      <c r="C19" s="289"/>
+      <c r="D19" s="282"/>
+      <c r="E19" s="283"/>
+      <c r="F19" s="185">
         <v>2</v>
       </c>
-      <c r="G19" s="238"/>
-      <c r="H19" s="238"/>
-      <c r="I19" s="238"/>
-      <c r="J19" s="238"/>
-      <c r="K19" s="238"/>
-      <c r="L19" s="238"/>
-      <c r="M19" s="239"/>
+      <c r="G19" s="186"/>
+      <c r="H19" s="186"/>
+      <c r="I19" s="186"/>
+      <c r="J19" s="186"/>
+      <c r="K19" s="186"/>
+      <c r="L19" s="186"/>
+      <c r="M19" s="187"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="242"/>
-      <c r="C20" s="243"/>
-      <c r="D20" s="233"/>
-      <c r="E20" s="234"/>
-      <c r="F20" s="237">
+      <c r="B20" s="288"/>
+      <c r="C20" s="289"/>
+      <c r="D20" s="282"/>
+      <c r="E20" s="283"/>
+      <c r="F20" s="185">
         <v>3</v>
       </c>
-      <c r="G20" s="238"/>
-      <c r="H20" s="238"/>
-      <c r="I20" s="238"/>
-      <c r="J20" s="238"/>
-      <c r="K20" s="238"/>
-      <c r="L20" s="238"/>
-      <c r="M20" s="239"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="186"/>
+      <c r="K20" s="186"/>
+      <c r="L20" s="186"/>
+      <c r="M20" s="187"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="244"/>
-      <c r="C21" s="245"/>
-      <c r="D21" s="235"/>
-      <c r="E21" s="236"/>
-      <c r="F21" s="237">
+      <c r="B21" s="290"/>
+      <c r="C21" s="291"/>
+      <c r="D21" s="284"/>
+      <c r="E21" s="285"/>
+      <c r="F21" s="185">
         <v>4</v>
       </c>
-      <c r="G21" s="238"/>
-      <c r="H21" s="238"/>
-      <c r="I21" s="238"/>
-      <c r="J21" s="238"/>
-      <c r="K21" s="238"/>
-      <c r="L21" s="238"/>
-      <c r="M21" s="239"/>
+      <c r="G21" s="186"/>
+      <c r="H21" s="186"/>
+      <c r="I21" s="186"/>
+      <c r="J21" s="186"/>
+      <c r="K21" s="186"/>
+      <c r="L21" s="186"/>
+      <c r="M21" s="187"/>
     </row>
     <row r="22" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="175" t="s">
+      <c r="B22" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="176"/>
-      <c r="D22" s="200" t="s">
+      <c r="C22" s="254"/>
+      <c r="D22" s="218" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="200"/>
-      <c r="F22" s="185"/>
-      <c r="G22" s="185"/>
-      <c r="H22" s="185"/>
-      <c r="I22" s="185"/>
-      <c r="J22" s="185"/>
-      <c r="K22" s="185"/>
-      <c r="L22" s="185"/>
-      <c r="M22" s="186"/>
+      <c r="E22" s="218"/>
+      <c r="F22" s="183"/>
+      <c r="G22" s="183"/>
+      <c r="H22" s="183"/>
+      <c r="I22" s="183"/>
+      <c r="J22" s="183"/>
+      <c r="K22" s="183"/>
+      <c r="L22" s="183"/>
+      <c r="M22" s="184"/>
     </row>
     <row r="23" spans="2:13" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="201" t="s">
+      <c r="B23" s="293" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="202"/>
-      <c r="D23" s="226" t="s">
+      <c r="C23" s="294"/>
+      <c r="D23" s="314" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="226"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
-      <c r="K23" s="206"/>
-      <c r="L23" s="206"/>
-      <c r="M23" s="207"/>
+      <c r="E23" s="314"/>
+      <c r="F23" s="296"/>
+      <c r="G23" s="296"/>
+      <c r="H23" s="296"/>
+      <c r="I23" s="296"/>
+      <c r="J23" s="296"/>
+      <c r="K23" s="296"/>
+      <c r="L23" s="296"/>
+      <c r="M23" s="297"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="208" t="s">
+      <c r="B24" s="298" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="209"/>
-      <c r="D24" s="209"/>
-      <c r="E24" s="209"/>
-      <c r="F24" s="209"/>
-      <c r="G24" s="209"/>
-      <c r="H24" s="209"/>
-      <c r="I24" s="209"/>
-      <c r="J24" s="209"/>
-      <c r="K24" s="209"/>
-      <c r="L24" s="209"/>
-      <c r="M24" s="210"/>
+      <c r="C24" s="299"/>
+      <c r="D24" s="299"/>
+      <c r="E24" s="299"/>
+      <c r="F24" s="299"/>
+      <c r="G24" s="299"/>
+      <c r="H24" s="299"/>
+      <c r="I24" s="299"/>
+      <c r="J24" s="299"/>
+      <c r="K24" s="299"/>
+      <c r="L24" s="299"/>
+      <c r="M24" s="300"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="211"/>
-      <c r="C25" s="212"/>
-      <c r="D25" s="212"/>
-      <c r="E25" s="212"/>
-      <c r="F25" s="212"/>
-      <c r="G25" s="212"/>
-      <c r="H25" s="212"/>
-      <c r="I25" s="212"/>
-      <c r="J25" s="212"/>
-      <c r="K25" s="212"/>
-      <c r="L25" s="212"/>
-      <c r="M25" s="213"/>
+      <c r="B25" s="301"/>
+      <c r="C25" s="302"/>
+      <c r="D25" s="302"/>
+      <c r="E25" s="302"/>
+      <c r="F25" s="302"/>
+      <c r="G25" s="302"/>
+      <c r="H25" s="302"/>
+      <c r="I25" s="302"/>
+      <c r="J25" s="302"/>
+      <c r="K25" s="302"/>
+      <c r="L25" s="302"/>
+      <c r="M25" s="303"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="214"/>
-      <c r="C26" s="215"/>
-      <c r="D26" s="215"/>
-      <c r="E26" s="215"/>
-      <c r="F26" s="215"/>
-      <c r="G26" s="215"/>
-      <c r="H26" s="215"/>
-      <c r="I26" s="215"/>
-      <c r="J26" s="215"/>
-      <c r="K26" s="215"/>
-      <c r="L26" s="215"/>
-      <c r="M26" s="216"/>
+      <c r="B26" s="304"/>
+      <c r="C26" s="305"/>
+      <c r="D26" s="305"/>
+      <c r="E26" s="305"/>
+      <c r="F26" s="305"/>
+      <c r="G26" s="305"/>
+      <c r="H26" s="305"/>
+      <c r="I26" s="305"/>
+      <c r="J26" s="305"/>
+      <c r="K26" s="305"/>
+      <c r="L26" s="305"/>
+      <c r="M26" s="306"/>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="217"/>
-      <c r="C27" s="218"/>
-      <c r="D27" s="218"/>
-      <c r="E27" s="218"/>
-      <c r="F27" s="218"/>
-      <c r="G27" s="218"/>
-      <c r="H27" s="218"/>
-      <c r="I27" s="218"/>
-      <c r="J27" s="218"/>
-      <c r="K27" s="218"/>
-      <c r="L27" s="218"/>
-      <c r="M27" s="219"/>
+      <c r="B27" s="307"/>
+      <c r="C27" s="308"/>
+      <c r="D27" s="308"/>
+      <c r="E27" s="308"/>
+      <c r="F27" s="308"/>
+      <c r="G27" s="308"/>
+      <c r="H27" s="308"/>
+      <c r="I27" s="308"/>
+      <c r="J27" s="308"/>
+      <c r="K27" s="308"/>
+      <c r="L27" s="308"/>
+      <c r="M27" s="309"/>
     </row>
     <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="261" t="s">
+      <c r="B28" s="257" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="262"/>
-      <c r="D28" s="262"/>
-      <c r="E28" s="262"/>
-      <c r="F28" s="262"/>
-      <c r="G28" s="262"/>
-      <c r="H28" s="262"/>
-      <c r="I28" s="262"/>
-      <c r="J28" s="262"/>
-      <c r="K28" s="262"/>
-      <c r="L28" s="262"/>
-      <c r="M28" s="263"/>
+      <c r="C28" s="258"/>
+      <c r="D28" s="258"/>
+      <c r="E28" s="258"/>
+      <c r="F28" s="258"/>
+      <c r="G28" s="258"/>
+      <c r="H28" s="258"/>
+      <c r="I28" s="258"/>
+      <c r="J28" s="258"/>
+      <c r="K28" s="258"/>
+      <c r="L28" s="258"/>
+      <c r="M28" s="259"/>
     </row>
     <row r="29" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="264" t="s">
+      <c r="B29" s="260" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="265"/>
-      <c r="D29" s="266"/>
-      <c r="E29" s="273" t="s">
+      <c r="C29" s="261"/>
+      <c r="D29" s="262"/>
+      <c r="E29" s="269" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="301"/>
-      <c r="G29" s="301"/>
-      <c r="H29" s="301"/>
-      <c r="I29" s="301"/>
-      <c r="J29" s="301"/>
-      <c r="K29" s="301"/>
-      <c r="L29" s="301"/>
-      <c r="M29" s="302"/>
+      <c r="F29" s="194"/>
+      <c r="G29" s="194"/>
+      <c r="H29" s="194"/>
+      <c r="I29" s="194"/>
+      <c r="J29" s="194"/>
+      <c r="K29" s="194"/>
+      <c r="L29" s="194"/>
+      <c r="M29" s="195"/>
     </row>
     <row r="30" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="267"/>
-      <c r="C30" s="268"/>
-      <c r="D30" s="269"/>
-      <c r="E30" s="203"/>
-      <c r="F30" s="303"/>
-      <c r="G30" s="303"/>
-      <c r="H30" s="303"/>
-      <c r="I30" s="303"/>
-      <c r="J30" s="303"/>
-      <c r="K30" s="303"/>
-      <c r="L30" s="303"/>
-      <c r="M30" s="304"/>
+      <c r="B30" s="263"/>
+      <c r="C30" s="264"/>
+      <c r="D30" s="265"/>
+      <c r="E30" s="270"/>
+      <c r="F30" s="196"/>
+      <c r="G30" s="196"/>
+      <c r="H30" s="196"/>
+      <c r="I30" s="196"/>
+      <c r="J30" s="196"/>
+      <c r="K30" s="196"/>
+      <c r="L30" s="196"/>
+      <c r="M30" s="197"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="270"/>
-      <c r="C31" s="271"/>
-      <c r="D31" s="272"/>
-      <c r="E31" s="204"/>
-      <c r="F31" s="305"/>
-      <c r="G31" s="305"/>
-      <c r="H31" s="305"/>
-      <c r="I31" s="305"/>
-      <c r="J31" s="305"/>
-      <c r="K31" s="305"/>
-      <c r="L31" s="305"/>
-      <c r="M31" s="306"/>
+      <c r="B31" s="266"/>
+      <c r="C31" s="267"/>
+      <c r="D31" s="268"/>
+      <c r="E31" s="271"/>
+      <c r="F31" s="198"/>
+      <c r="G31" s="198"/>
+      <c r="H31" s="198"/>
+      <c r="I31" s="198"/>
+      <c r="J31" s="198"/>
+      <c r="K31" s="198"/>
+      <c r="L31" s="198"/>
+      <c r="M31" s="199"/>
     </row>
     <row r="32" spans="2:13" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="274" t="s">
+      <c r="B32" s="272" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="275"/>
-      <c r="D32" s="276"/>
+      <c r="C32" s="273"/>
+      <c r="D32" s="274"/>
       <c r="E32" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="277"/>
-      <c r="G32" s="277"/>
-      <c r="H32" s="277"/>
-      <c r="I32" s="277"/>
-      <c r="J32" s="277"/>
-      <c r="K32" s="277"/>
-      <c r="L32" s="277"/>
-      <c r="M32" s="278"/>
+      <c r="F32" s="275"/>
+      <c r="G32" s="275"/>
+      <c r="H32" s="275"/>
+      <c r="I32" s="275"/>
+      <c r="J32" s="275"/>
+      <c r="K32" s="275"/>
+      <c r="L32" s="275"/>
+      <c r="M32" s="276"/>
     </row>
     <row r="33" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="267" t="s">
+      <c r="B33" s="263" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="268"/>
-      <c r="D33" s="269"/>
-      <c r="E33" s="203" t="s">
+      <c r="C33" s="264"/>
+      <c r="D33" s="265"/>
+      <c r="E33" s="270" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="224" t="s">
+      <c r="F33" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="224"/>
-      <c r="H33" s="224"/>
-      <c r="I33" s="224"/>
-      <c r="J33" s="224"/>
-      <c r="K33" s="224" t="s">
+      <c r="G33" s="220"/>
+      <c r="H33" s="220"/>
+      <c r="I33" s="220"/>
+      <c r="J33" s="220"/>
+      <c r="K33" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="L33" s="224"/>
-      <c r="M33" s="225"/>
+      <c r="L33" s="220"/>
+      <c r="M33" s="313"/>
     </row>
     <row r="34" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="270"/>
-      <c r="C34" s="271"/>
-      <c r="D34" s="272"/>
-      <c r="E34" s="204"/>
-      <c r="F34" s="289" t="s">
+      <c r="B34" s="266"/>
+      <c r="C34" s="267"/>
+      <c r="D34" s="268"/>
+      <c r="E34" s="271"/>
+      <c r="F34" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="289"/>
-      <c r="H34" s="289"/>
-      <c r="I34" s="289"/>
-      <c r="J34" s="289"/>
-      <c r="K34" s="222"/>
-      <c r="L34" s="222"/>
-      <c r="M34" s="223"/>
+      <c r="G34" s="221"/>
+      <c r="H34" s="221"/>
+      <c r="I34" s="221"/>
+      <c r="J34" s="221"/>
+      <c r="K34" s="311"/>
+      <c r="L34" s="311"/>
+      <c r="M34" s="312"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="270"/>
-      <c r="C35" s="271"/>
-      <c r="D35" s="272"/>
-      <c r="E35" s="204"/>
-      <c r="F35" s="286" t="s">
+      <c r="B35" s="266"/>
+      <c r="C35" s="267"/>
+      <c r="D35" s="268"/>
+      <c r="E35" s="271"/>
+      <c r="F35" s="222" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="286"/>
-      <c r="H35" s="286"/>
-      <c r="I35" s="286"/>
-      <c r="J35" s="286"/>
-      <c r="K35" s="227"/>
-      <c r="L35" s="228"/>
-      <c r="M35" s="229"/>
+      <c r="G35" s="222"/>
+      <c r="H35" s="222"/>
+      <c r="I35" s="222"/>
+      <c r="J35" s="222"/>
+      <c r="K35" s="224"/>
+      <c r="L35" s="225"/>
+      <c r="M35" s="226"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="270"/>
-      <c r="C36" s="271"/>
-      <c r="D36" s="272"/>
-      <c r="E36" s="204"/>
-      <c r="F36" s="227" t="s">
+      <c r="B36" s="266"/>
+      <c r="C36" s="267"/>
+      <c r="D36" s="268"/>
+      <c r="E36" s="271"/>
+      <c r="F36" s="224" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="228"/>
-      <c r="H36" s="228"/>
-      <c r="I36" s="228"/>
-      <c r="J36" s="230"/>
-      <c r="K36" s="227"/>
-      <c r="L36" s="228"/>
-      <c r="M36" s="229"/>
+      <c r="G36" s="225"/>
+      <c r="H36" s="225"/>
+      <c r="I36" s="225"/>
+      <c r="J36" s="315"/>
+      <c r="K36" s="224"/>
+      <c r="L36" s="225"/>
+      <c r="M36" s="226"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="270"/>
-      <c r="C37" s="271"/>
-      <c r="D37" s="272"/>
-      <c r="E37" s="204"/>
-      <c r="F37" s="286" t="s">
+      <c r="B37" s="266"/>
+      <c r="C37" s="267"/>
+      <c r="D37" s="268"/>
+      <c r="E37" s="271"/>
+      <c r="F37" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="286"/>
-      <c r="H37" s="286"/>
-      <c r="I37" s="286"/>
-      <c r="J37" s="286"/>
-      <c r="K37" s="286"/>
-      <c r="L37" s="286"/>
-      <c r="M37" s="287"/>
+      <c r="G37" s="222"/>
+      <c r="H37" s="222"/>
+      <c r="I37" s="222"/>
+      <c r="J37" s="222"/>
+      <c r="K37" s="222"/>
+      <c r="L37" s="222"/>
+      <c r="M37" s="240"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B38" s="270"/>
-      <c r="C38" s="271"/>
-      <c r="D38" s="272"/>
-      <c r="E38" s="204"/>
-      <c r="F38" s="286" t="s">
+      <c r="B38" s="266"/>
+      <c r="C38" s="267"/>
+      <c r="D38" s="268"/>
+      <c r="E38" s="271"/>
+      <c r="F38" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="286"/>
-      <c r="H38" s="286"/>
-      <c r="I38" s="286"/>
-      <c r="J38" s="286"/>
-      <c r="K38" s="286"/>
-      <c r="L38" s="286"/>
-      <c r="M38" s="287"/>
+      <c r="G38" s="222"/>
+      <c r="H38" s="222"/>
+      <c r="I38" s="222"/>
+      <c r="J38" s="222"/>
+      <c r="K38" s="222"/>
+      <c r="L38" s="222"/>
+      <c r="M38" s="240"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B39" s="270"/>
-      <c r="C39" s="271"/>
-      <c r="D39" s="272"/>
-      <c r="E39" s="204"/>
-      <c r="F39" s="286" t="s">
+      <c r="B39" s="266"/>
+      <c r="C39" s="267"/>
+      <c r="D39" s="268"/>
+      <c r="E39" s="271"/>
+      <c r="F39" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="286"/>
-      <c r="H39" s="286"/>
-      <c r="I39" s="286"/>
-      <c r="J39" s="286"/>
-      <c r="K39" s="286"/>
-      <c r="L39" s="286"/>
-      <c r="M39" s="287"/>
+      <c r="G39" s="222"/>
+      <c r="H39" s="222"/>
+      <c r="I39" s="222"/>
+      <c r="J39" s="222"/>
+      <c r="K39" s="222"/>
+      <c r="L39" s="222"/>
+      <c r="M39" s="240"/>
     </row>
     <row r="40" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="279"/>
-      <c r="C40" s="280"/>
-      <c r="D40" s="281"/>
-      <c r="E40" s="205"/>
-      <c r="F40" s="220" t="s">
+      <c r="B40" s="277"/>
+      <c r="C40" s="278"/>
+      <c r="D40" s="279"/>
+      <c r="E40" s="295"/>
+      <c r="F40" s="223" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="220"/>
-      <c r="H40" s="220"/>
-      <c r="I40" s="220"/>
-      <c r="J40" s="220"/>
-      <c r="K40" s="220"/>
-      <c r="L40" s="220"/>
-      <c r="M40" s="221"/>
+      <c r="G40" s="223"/>
+      <c r="H40" s="223"/>
+      <c r="I40" s="223"/>
+      <c r="J40" s="223"/>
+      <c r="K40" s="223"/>
+      <c r="L40" s="223"/>
+      <c r="M40" s="310"/>
     </row>
     <row r="41" spans="2:13" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="250" t="s">
+      <c r="B41" s="245" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="251"/>
-      <c r="D41" s="252"/>
+      <c r="C41" s="246"/>
+      <c r="D41" s="247"/>
       <c r="E41" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="293"/>
-      <c r="G41" s="293"/>
-      <c r="H41" s="293"/>
-      <c r="I41" s="293"/>
-      <c r="J41" s="293"/>
-      <c r="K41" s="293"/>
-      <c r="L41" s="293"/>
-      <c r="M41" s="294"/>
+      <c r="F41" s="232"/>
+      <c r="G41" s="232"/>
+      <c r="H41" s="232"/>
+      <c r="I41" s="232"/>
+      <c r="J41" s="232"/>
+      <c r="K41" s="232"/>
+      <c r="L41" s="232"/>
+      <c r="M41" s="233"/>
     </row>
     <row r="42" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="179" t="s">
+      <c r="B42" s="248" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="180"/>
-      <c r="D42" s="180"/>
-      <c r="E42" s="180"/>
-      <c r="F42" s="180"/>
-      <c r="G42" s="180"/>
-      <c r="H42" s="180"/>
-      <c r="I42" s="180"/>
-      <c r="J42" s="180"/>
-      <c r="K42" s="180"/>
-      <c r="L42" s="180"/>
-      <c r="M42" s="181"/>
+      <c r="C42" s="249"/>
+      <c r="D42" s="249"/>
+      <c r="E42" s="249"/>
+      <c r="F42" s="249"/>
+      <c r="G42" s="249"/>
+      <c r="H42" s="249"/>
+      <c r="I42" s="249"/>
+      <c r="J42" s="249"/>
+      <c r="K42" s="249"/>
+      <c r="L42" s="249"/>
+      <c r="M42" s="250"/>
     </row>
     <row r="43" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="253" t="s">
+      <c r="B43" s="251" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="254"/>
-      <c r="D43" s="255"/>
-      <c r="E43" s="255"/>
-      <c r="F43" s="284" t="s">
+      <c r="C43" s="239"/>
+      <c r="D43" s="252"/>
+      <c r="E43" s="252"/>
+      <c r="F43" s="237" t="s">
         <v>88</v>
       </c>
-      <c r="G43" s="285"/>
-      <c r="H43" s="285"/>
-      <c r="I43" s="285"/>
-      <c r="J43" s="285"/>
-      <c r="K43" s="254"/>
-      <c r="L43" s="255" t="s">
+      <c r="G43" s="238"/>
+      <c r="H43" s="238"/>
+      <c r="I43" s="238"/>
+      <c r="J43" s="238"/>
+      <c r="K43" s="239"/>
+      <c r="L43" s="252" t="s">
         <v>28</v>
       </c>
-      <c r="M43" s="260"/>
+      <c r="M43" s="256"/>
     </row>
     <row r="44" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="256" t="s">
+      <c r="B44" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="176"/>
-      <c r="D44" s="257"/>
-      <c r="E44" s="257"/>
-      <c r="F44" s="283"/>
-      <c r="G44" s="283"/>
-      <c r="H44" s="283"/>
-      <c r="I44" s="283"/>
-      <c r="J44" s="283"/>
-      <c r="K44" s="283"/>
-      <c r="L44" s="283"/>
-      <c r="M44" s="290"/>
+      <c r="C44" s="254"/>
+      <c r="D44" s="255"/>
+      <c r="E44" s="255"/>
+      <c r="F44" s="227"/>
+      <c r="G44" s="227"/>
+      <c r="H44" s="227"/>
+      <c r="I44" s="227"/>
+      <c r="J44" s="227"/>
+      <c r="K44" s="227"/>
+      <c r="L44" s="227"/>
+      <c r="M44" s="228"/>
     </row>
     <row r="45" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="258" t="s">
+      <c r="B45" s="234" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="178"/>
-      <c r="D45" s="259"/>
-      <c r="E45" s="259"/>
-      <c r="F45" s="282"/>
-      <c r="G45" s="282"/>
-      <c r="H45" s="282"/>
-      <c r="I45" s="282"/>
-      <c r="J45" s="282"/>
-      <c r="K45" s="282"/>
-      <c r="L45" s="282"/>
-      <c r="M45" s="291"/>
+      <c r="C45" s="235"/>
+      <c r="D45" s="236"/>
+      <c r="E45" s="236"/>
+      <c r="F45" s="229"/>
+      <c r="G45" s="229"/>
+      <c r="H45" s="229"/>
+      <c r="I45" s="229"/>
+      <c r="J45" s="229"/>
+      <c r="K45" s="229"/>
+      <c r="L45" s="229"/>
+      <c r="M45" s="230"/>
     </row>
     <row r="46" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="256" t="s">
+      <c r="B46" s="253" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="176"/>
-      <c r="D46" s="257"/>
-      <c r="E46" s="257"/>
-      <c r="F46" s="283"/>
-      <c r="G46" s="283"/>
-      <c r="H46" s="283"/>
-      <c r="I46" s="283"/>
-      <c r="J46" s="283"/>
-      <c r="K46" s="283"/>
-      <c r="L46" s="283"/>
-      <c r="M46" s="290"/>
+      <c r="C46" s="254"/>
+      <c r="D46" s="255"/>
+      <c r="E46" s="255"/>
+      <c r="F46" s="227"/>
+      <c r="G46" s="227"/>
+      <c r="H46" s="227"/>
+      <c r="I46" s="227"/>
+      <c r="J46" s="227"/>
+      <c r="K46" s="227"/>
+      <c r="L46" s="227"/>
+      <c r="M46" s="228"/>
     </row>
     <row r="47" spans="2:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="258" t="s">
+      <c r="B47" s="234" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="178"/>
-      <c r="D47" s="259"/>
-      <c r="E47" s="259"/>
-      <c r="F47" s="282"/>
-      <c r="G47" s="282"/>
-      <c r="H47" s="282"/>
-      <c r="I47" s="282"/>
-      <c r="J47" s="282"/>
-      <c r="K47" s="282"/>
-      <c r="L47" s="282"/>
-      <c r="M47" s="291"/>
+      <c r="C47" s="235"/>
+      <c r="D47" s="236"/>
+      <c r="E47" s="236"/>
+      <c r="F47" s="229"/>
+      <c r="G47" s="229"/>
+      <c r="H47" s="229"/>
+      <c r="I47" s="229"/>
+      <c r="J47" s="229"/>
+      <c r="K47" s="229"/>
+      <c r="L47" s="229"/>
+      <c r="M47" s="230"/>
     </row>
     <row r="48" spans="2:13" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="246" t="s">
+      <c r="B48" s="241" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="247"/>
-      <c r="D48" s="248"/>
-      <c r="E48" s="248"/>
-      <c r="F48" s="288"/>
-      <c r="G48" s="288"/>
-      <c r="H48" s="288"/>
-      <c r="I48" s="288"/>
-      <c r="J48" s="288"/>
-      <c r="K48" s="288"/>
-      <c r="L48" s="288"/>
-      <c r="M48" s="292"/>
+      <c r="C48" s="242"/>
+      <c r="D48" s="243"/>
+      <c r="E48" s="243"/>
+      <c r="F48" s="219"/>
+      <c r="G48" s="219"/>
+      <c r="H48" s="219"/>
+      <c r="I48" s="219"/>
+      <c r="J48" s="219"/>
+      <c r="K48" s="219"/>
+      <c r="L48" s="219"/>
+      <c r="M48" s="231"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="156"/>
@@ -5644,6 +5644,79 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:M14"/>
+    <mergeCell ref="F15:M15"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F11:M11"/>
+    <mergeCell ref="F12:M12"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E33:E40"/>
+    <mergeCell ref="F23:M23"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B25:M27"/>
+    <mergeCell ref="F22:M22"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="D18:E21"/>
+    <mergeCell ref="F19:M19"/>
+    <mergeCell ref="F20:M20"/>
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="B18:C21"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:M42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="B33:D40"/>
+    <mergeCell ref="F45:K45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="F44:K44"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="F48:K48"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="F35:J35"/>
+    <mergeCell ref="F37:J37"/>
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="F39:J39"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="F47:K47"/>
+    <mergeCell ref="F41:M41"/>
     <mergeCell ref="F17:M17"/>
     <mergeCell ref="F18:M18"/>
     <mergeCell ref="B2:M3"/>
@@ -5660,79 +5733,6 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F48:K48"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="F35:J35"/>
-    <mergeCell ref="F37:J37"/>
-    <mergeCell ref="F38:J38"/>
-    <mergeCell ref="F39:J39"/>
-    <mergeCell ref="F40:J40"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="F47:K47"/>
-    <mergeCell ref="F41:M41"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="F44:K44"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:M42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="B33:D40"/>
-    <mergeCell ref="F45:K45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="D18:E21"/>
-    <mergeCell ref="F19:M19"/>
-    <mergeCell ref="F20:M20"/>
-    <mergeCell ref="F21:M21"/>
-    <mergeCell ref="B18:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E33:E40"/>
-    <mergeCell ref="F23:M23"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B25:M27"/>
-    <mergeCell ref="F22:M22"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:M14"/>
-    <mergeCell ref="F15:M15"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F11:M11"/>
-    <mergeCell ref="F12:M12"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:M16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" r:id="rId1"/>
@@ -5795,21 +5795,21 @@
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="147"/>
-      <c r="C2" s="322" t="s">
+      <c r="C2" s="334" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="322"/>
-      <c r="E2" s="322"/>
-      <c r="F2" s="322"/>
-      <c r="G2" s="322"/>
-      <c r="H2" s="322"/>
-      <c r="I2" s="322"/>
-      <c r="J2" s="322"/>
-      <c r="K2" s="322"/>
-      <c r="L2" s="322"/>
-      <c r="M2" s="322"/>
-      <c r="N2" s="322"/>
-      <c r="O2" s="322"/>
+      <c r="D2" s="334"/>
+      <c r="E2" s="334"/>
+      <c r="F2" s="334"/>
+      <c r="G2" s="334"/>
+      <c r="H2" s="334"/>
+      <c r="I2" s="334"/>
+      <c r="J2" s="334"/>
+      <c r="K2" s="334"/>
+      <c r="L2" s="334"/>
+      <c r="M2" s="334"/>
+      <c r="N2" s="334"/>
+      <c r="O2" s="334"/>
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" s="8" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5833,23 +5833,23 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="148"/>
-      <c r="C4" s="323" t="s">
+      <c r="C4" s="335" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
-      <c r="G4" s="323"/>
-      <c r="H4" s="323"/>
-      <c r="I4" s="323"/>
-      <c r="J4" s="323"/>
-      <c r="K4" s="323"/>
-      <c r="L4" s="323"/>
-      <c r="M4" s="323"/>
-      <c r="N4" s="323"/>
-      <c r="O4" s="323"/>
-      <c r="P4" s="323"/>
-      <c r="Q4" s="323"/>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="335"/>
+      <c r="G4" s="335"/>
+      <c r="H4" s="335"/>
+      <c r="I4" s="335"/>
+      <c r="J4" s="335"/>
+      <c r="K4" s="335"/>
+      <c r="L4" s="335"/>
+      <c r="M4" s="335"/>
+      <c r="N4" s="335"/>
+      <c r="O4" s="335"/>
+      <c r="P4" s="335"/>
+      <c r="Q4" s="335"/>
       <c r="R4" s="11"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -5881,13 +5881,13 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="324"/>
-      <c r="J6" s="324"/>
-      <c r="K6" s="324"/>
-      <c r="L6" s="324"/>
-      <c r="M6" s="324"/>
-      <c r="N6" s="324"/>
-      <c r="O6" s="324"/>
+      <c r="I6" s="336"/>
+      <c r="J6" s="336"/>
+      <c r="K6" s="336"/>
+      <c r="L6" s="336"/>
+      <c r="M6" s="336"/>
+      <c r="N6" s="336"/>
+      <c r="O6" s="336"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="11"/>
@@ -6302,8 +6302,8 @@
   </sheetPr>
   <dimension ref="B1:AI66"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6330,26 +6330,26 @@
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="28"/>
-      <c r="E2" s="373" t="s">
+      <c r="E2" s="374" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="374"/>
-      <c r="G2" s="374"/>
-      <c r="H2" s="374"/>
-      <c r="I2" s="374"/>
-      <c r="J2" s="374"/>
-      <c r="K2" s="374"/>
-      <c r="L2" s="374"/>
-      <c r="M2" s="374"/>
-      <c r="N2" s="374"/>
-      <c r="O2" s="374"/>
-      <c r="P2" s="374"/>
-      <c r="Q2" s="374"/>
-      <c r="R2" s="374"/>
-      <c r="S2" s="374"/>
-      <c r="T2" s="374"/>
-      <c r="U2" s="374"/>
-      <c r="V2" s="374"/>
+      <c r="F2" s="375"/>
+      <c r="G2" s="375"/>
+      <c r="H2" s="375"/>
+      <c r="I2" s="375"/>
+      <c r="J2" s="375"/>
+      <c r="K2" s="375"/>
+      <c r="L2" s="375"/>
+      <c r="M2" s="375"/>
+      <c r="N2" s="375"/>
+      <c r="O2" s="375"/>
+      <c r="P2" s="375"/>
+      <c r="Q2" s="375"/>
+      <c r="R2" s="375"/>
+      <c r="S2" s="375"/>
+      <c r="T2" s="375"/>
+      <c r="U2" s="375"/>
+      <c r="V2" s="375"/>
       <c r="W2" s="29"/>
       <c r="X2" s="132"/>
       <c r="Y2" s="132" t="s">
@@ -6357,12 +6357,12 @@
       </c>
       <c r="Z2" s="132"/>
       <c r="AA2" s="133"/>
-      <c r="AB2" s="369" t="s">
+      <c r="AB2" s="362" t="s">
         <v>108</v>
       </c>
-      <c r="AC2" s="369"/>
-      <c r="AD2" s="369"/>
-      <c r="AE2" s="370"/>
+      <c r="AC2" s="362"/>
+      <c r="AD2" s="362"/>
+      <c r="AE2" s="363"/>
       <c r="AG2" s="30"/>
       <c r="AH2" s="31"/>
       <c r="AI2" s="31"/>
@@ -6374,37 +6374,37 @@
       <c r="F3" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="375" t="s">
+      <c r="G3" s="351" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="375"/>
-      <c r="I3" s="375"/>
-      <c r="J3" s="375"/>
-      <c r="K3" s="385"/>
-      <c r="L3" s="385"/>
+      <c r="H3" s="351"/>
+      <c r="I3" s="351"/>
+      <c r="J3" s="351"/>
+      <c r="K3" s="172"/>
+      <c r="L3" s="172"/>
       <c r="M3" s="134"/>
-      <c r="N3" s="376" t="s">
+      <c r="N3" s="339" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="376"/>
-      <c r="P3" s="376"/>
-      <c r="Q3" s="376"/>
-      <c r="R3" s="376"/>
-      <c r="S3" s="375" t="s">
+      <c r="O3" s="339"/>
+      <c r="P3" s="339"/>
+      <c r="Q3" s="339"/>
+      <c r="R3" s="339"/>
+      <c r="S3" s="351" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="375"/>
-      <c r="U3" s="375"/>
-      <c r="V3" s="375"/>
-      <c r="W3" s="375"/>
-      <c r="X3" s="375"/>
-      <c r="Y3" s="375"/>
-      <c r="Z3" s="375"/>
-      <c r="AA3" s="375"/>
-      <c r="AB3" s="375"/>
-      <c r="AC3" s="375"/>
-      <c r="AD3" s="366"/>
-      <c r="AE3" s="367"/>
+      <c r="T3" s="351"/>
+      <c r="U3" s="351"/>
+      <c r="V3" s="351"/>
+      <c r="W3" s="351"/>
+      <c r="X3" s="351"/>
+      <c r="Y3" s="351"/>
+      <c r="Z3" s="351"/>
+      <c r="AA3" s="351"/>
+      <c r="AB3" s="351"/>
+      <c r="AC3" s="351"/>
+      <c r="AD3" s="357"/>
+      <c r="AE3" s="358"/>
       <c r="AG3" s="30"/>
       <c r="AH3" s="31"/>
       <c r="AI3" s="31"/>
@@ -6416,33 +6416,33 @@
       <c r="F4" s="110" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="382" t="s">
+      <c r="G4" s="355" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="382"/>
-      <c r="I4" s="382"/>
-      <c r="J4" s="382"/>
-      <c r="K4" s="386"/>
-      <c r="L4" s="386"/>
+      <c r="H4" s="355"/>
+      <c r="I4" s="355"/>
+      <c r="J4" s="355"/>
+      <c r="K4" s="173"/>
+      <c r="L4" s="173"/>
       <c r="M4" s="135"/>
-      <c r="N4" s="377" t="s">
+      <c r="N4" s="343" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="377"/>
-      <c r="P4" s="377"/>
-      <c r="Q4" s="377"/>
-      <c r="R4" s="377"/>
-      <c r="S4" s="375"/>
-      <c r="T4" s="375"/>
-      <c r="U4" s="375"/>
-      <c r="V4" s="375"/>
-      <c r="W4" s="375"/>
-      <c r="X4" s="375"/>
-      <c r="Y4" s="375"/>
-      <c r="Z4" s="375"/>
-      <c r="AA4" s="375"/>
-      <c r="AB4" s="375"/>
-      <c r="AC4" s="375"/>
+      <c r="O4" s="343"/>
+      <c r="P4" s="343"/>
+      <c r="Q4" s="343"/>
+      <c r="R4" s="343"/>
+      <c r="S4" s="351"/>
+      <c r="T4" s="351"/>
+      <c r="U4" s="351"/>
+      <c r="V4" s="351"/>
+      <c r="W4" s="351"/>
+      <c r="X4" s="351"/>
+      <c r="Y4" s="351"/>
+      <c r="Z4" s="351"/>
+      <c r="AA4" s="351"/>
+      <c r="AB4" s="351"/>
+      <c r="AC4" s="351"/>
       <c r="AD4" s="134"/>
       <c r="AE4" s="136"/>
       <c r="AG4" s="30"/>
@@ -6455,24 +6455,24 @@
       <c r="D5" s="36"/>
       <c r="E5" s="107"/>
       <c r="F5" s="108"/>
-      <c r="G5" s="383"/>
-      <c r="H5" s="383"/>
-      <c r="I5" s="383"/>
-      <c r="J5" s="383"/>
+      <c r="G5" s="356"/>
+      <c r="H5" s="356"/>
+      <c r="I5" s="356"/>
+      <c r="J5" s="356"/>
       <c r="K5" s="170"/>
       <c r="L5" s="170"/>
       <c r="M5" s="137"/>
-      <c r="N5" s="378" t="s">
+      <c r="N5" s="344" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="378"/>
-      <c r="P5" s="378"/>
-      <c r="Q5" s="378"/>
-      <c r="R5" s="378"/>
-      <c r="S5" s="372"/>
-      <c r="T5" s="372"/>
-      <c r="U5" s="372"/>
-      <c r="V5" s="372"/>
+      <c r="O5" s="344"/>
+      <c r="P5" s="344"/>
+      <c r="Q5" s="344"/>
+      <c r="R5" s="344"/>
+      <c r="S5" s="373"/>
+      <c r="T5" s="373"/>
+      <c r="U5" s="373"/>
+      <c r="V5" s="373"/>
       <c r="W5" s="137"/>
       <c r="X5" s="137"/>
       <c r="Y5" s="137"/>
@@ -6487,58 +6487,58 @@
       <c r="AI5" s="38"/>
     </row>
     <row r="6" spans="2:35" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="328" t="s">
+      <c r="B6" s="386" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="329"/>
-      <c r="D6" s="329"/>
+      <c r="C6" s="387"/>
+      <c r="D6" s="387"/>
       <c r="E6" s="111"/>
       <c r="F6" s="112" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="113"/>
       <c r="H6" s="114"/>
-      <c r="I6" s="341" t="s">
+      <c r="I6" s="388" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="342"/>
-      <c r="K6" s="342"/>
-      <c r="L6" s="342"/>
-      <c r="M6" s="342"/>
-      <c r="N6" s="342"/>
-      <c r="O6" s="342"/>
-      <c r="P6" s="342"/>
-      <c r="Q6" s="342"/>
-      <c r="R6" s="342"/>
-      <c r="S6" s="342"/>
-      <c r="T6" s="342"/>
-      <c r="U6" s="342"/>
-      <c r="V6" s="343"/>
-      <c r="W6" s="343"/>
-      <c r="X6" s="344"/>
-      <c r="Y6" s="368" t="s">
+      <c r="J6" s="360"/>
+      <c r="K6" s="360"/>
+      <c r="L6" s="360"/>
+      <c r="M6" s="360"/>
+      <c r="N6" s="360"/>
+      <c r="O6" s="360"/>
+      <c r="P6" s="360"/>
+      <c r="Q6" s="360"/>
+      <c r="R6" s="360"/>
+      <c r="S6" s="360"/>
+      <c r="T6" s="360"/>
+      <c r="U6" s="360"/>
+      <c r="V6" s="389"/>
+      <c r="W6" s="389"/>
+      <c r="X6" s="361"/>
+      <c r="Y6" s="359" t="s">
         <v>55</v>
       </c>
-      <c r="Z6" s="342"/>
-      <c r="AA6" s="342"/>
-      <c r="AB6" s="342"/>
-      <c r="AC6" s="342"/>
-      <c r="AD6" s="342"/>
-      <c r="AE6" s="344"/>
+      <c r="Z6" s="360"/>
+      <c r="AA6" s="360"/>
+      <c r="AB6" s="360"/>
+      <c r="AC6" s="360"/>
+      <c r="AD6" s="360"/>
+      <c r="AE6" s="361"/>
     </row>
     <row r="7" spans="2:35" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="40"/>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
-      <c r="E7" s="412">
+      <c r="E7" s="180">
         <v>1</v>
       </c>
-      <c r="F7" s="400" t="s">
+      <c r="F7" s="348" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="401"/>
-      <c r="H7" s="402"/>
-      <c r="I7" s="413"/>
+      <c r="G7" s="349"/>
+      <c r="H7" s="350"/>
+      <c r="I7" s="181"/>
       <c r="J7" s="43"/>
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
@@ -6569,15 +6569,15 @@
       <c r="B8" s="51"/>
       <c r="C8" s="52"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="412">
+      <c r="E8" s="180">
         <v>2</v>
       </c>
-      <c r="F8" s="403" t="s">
+      <c r="F8" s="345" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="404"/>
-      <c r="H8" s="405"/>
-      <c r="I8" s="414"/>
+      <c r="G8" s="346"/>
+      <c r="H8" s="347"/>
+      <c r="I8" s="182"/>
       <c r="J8" s="54"/>
       <c r="K8" s="54"/>
       <c r="L8" s="54"/>
@@ -6608,15 +6608,15 @@
       <c r="B9" s="51"/>
       <c r="C9" s="52"/>
       <c r="D9" s="53"/>
-      <c r="E9" s="412">
+      <c r="E9" s="180">
         <v>3</v>
       </c>
-      <c r="F9" s="403" t="s">
+      <c r="F9" s="345" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="404"/>
-      <c r="H9" s="405"/>
-      <c r="I9" s="414"/>
+      <c r="G9" s="346"/>
+      <c r="H9" s="347"/>
+      <c r="I9" s="182"/>
       <c r="J9" s="54"/>
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
@@ -6647,15 +6647,15 @@
       <c r="B10" s="51"/>
       <c r="C10" s="52"/>
       <c r="D10" s="53"/>
-      <c r="E10" s="412">
+      <c r="E10" s="180">
         <v>4</v>
       </c>
-      <c r="F10" s="403" t="s">
+      <c r="F10" s="345" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="404"/>
-      <c r="H10" s="405"/>
-      <c r="I10" s="414"/>
+      <c r="G10" s="346"/>
+      <c r="H10" s="347"/>
+      <c r="I10" s="182"/>
       <c r="J10" s="54"/>
       <c r="K10" s="54"/>
       <c r="L10" s="54"/>
@@ -6686,15 +6686,15 @@
       <c r="B11" s="51"/>
       <c r="C11" s="52"/>
       <c r="D11" s="53"/>
-      <c r="E11" s="412">
+      <c r="E11" s="180">
         <v>5</v>
       </c>
-      <c r="F11" s="403" t="s">
+      <c r="F11" s="345" t="s">
         <v>124</v>
       </c>
-      <c r="G11" s="404"/>
-      <c r="H11" s="405"/>
-      <c r="I11" s="414"/>
+      <c r="G11" s="346"/>
+      <c r="H11" s="347"/>
+      <c r="I11" s="182"/>
       <c r="J11" s="54"/>
       <c r="K11" s="54"/>
       <c r="L11" s="54"/>
@@ -6725,15 +6725,15 @@
       <c r="B12" s="51"/>
       <c r="C12" s="52"/>
       <c r="D12" s="53"/>
-      <c r="E12" s="412">
+      <c r="E12" s="180">
         <v>6</v>
       </c>
-      <c r="F12" s="403" t="s">
+      <c r="F12" s="345" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="404"/>
-      <c r="H12" s="405"/>
-      <c r="I12" s="414"/>
+      <c r="G12" s="346"/>
+      <c r="H12" s="347"/>
+      <c r="I12" s="182"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
@@ -6764,15 +6764,15 @@
       <c r="B13" s="51"/>
       <c r="C13" s="52"/>
       <c r="D13" s="53"/>
-      <c r="E13" s="412">
+      <c r="E13" s="180">
         <v>7</v>
       </c>
-      <c r="F13" s="403" t="s">
+      <c r="F13" s="345" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="404"/>
-      <c r="H13" s="405"/>
-      <c r="I13" s="414"/>
+      <c r="G13" s="346"/>
+      <c r="H13" s="347"/>
+      <c r="I13" s="182"/>
       <c r="J13" s="54"/>
       <c r="K13" s="54"/>
       <c r="L13" s="54"/>
@@ -6803,15 +6803,15 @@
       <c r="B14" s="51"/>
       <c r="C14" s="52"/>
       <c r="D14" s="53"/>
-      <c r="E14" s="412">
+      <c r="E14" s="180">
         <v>8</v>
       </c>
-      <c r="F14" s="403" t="s">
+      <c r="F14" s="345" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="404"/>
-      <c r="H14" s="405"/>
-      <c r="I14" s="414"/>
+      <c r="G14" s="346"/>
+      <c r="H14" s="347"/>
+      <c r="I14" s="182"/>
       <c r="J14" s="54"/>
       <c r="K14" s="54"/>
       <c r="L14" s="54"/>
@@ -6842,15 +6842,15 @@
       <c r="B15" s="51"/>
       <c r="C15" s="52"/>
       <c r="D15" s="53"/>
-      <c r="E15" s="412">
+      <c r="E15" s="180">
         <v>9</v>
       </c>
-      <c r="F15" s="403" t="s">
+      <c r="F15" s="345" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="404"/>
-      <c r="H15" s="405"/>
-      <c r="I15" s="414"/>
+      <c r="G15" s="346"/>
+      <c r="H15" s="347"/>
+      <c r="I15" s="182"/>
       <c r="J15" s="54"/>
       <c r="K15" s="54"/>
       <c r="L15" s="54"/>
@@ -6881,15 +6881,15 @@
       <c r="B16" s="51"/>
       <c r="C16" s="52"/>
       <c r="D16" s="53"/>
-      <c r="E16" s="412">
+      <c r="E16" s="180">
         <v>10</v>
       </c>
-      <c r="F16" s="406" t="s">
+      <c r="F16" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="407"/>
-      <c r="H16" s="408"/>
-      <c r="I16" s="414"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="176"/>
+      <c r="I16" s="182"/>
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
       <c r="L16" s="54"/>
@@ -6920,15 +6920,15 @@
       <c r="B17" s="51"/>
       <c r="C17" s="52"/>
       <c r="D17" s="53"/>
-      <c r="E17" s="412">
+      <c r="E17" s="180">
         <v>11</v>
       </c>
-      <c r="F17" s="403" t="s">
+      <c r="F17" s="345" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="404"/>
-      <c r="H17" s="405"/>
-      <c r="I17" s="414"/>
+      <c r="G17" s="346"/>
+      <c r="H17" s="347"/>
+      <c r="I17" s="182"/>
       <c r="J17" s="54"/>
       <c r="K17" s="54"/>
       <c r="L17" s="54"/>
@@ -6959,23 +6959,23 @@
       <c r="B18" s="51"/>
       <c r="C18" s="52"/>
       <c r="D18" s="53"/>
-      <c r="E18" s="412">
+      <c r="E18" s="180">
         <v>12</v>
       </c>
-      <c r="F18" s="403" t="s">
+      <c r="F18" s="345" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="404"/>
-      <c r="H18" s="405"/>
-      <c r="I18" s="414"/>
+      <c r="G18" s="346"/>
+      <c r="H18" s="347"/>
+      <c r="I18" s="182"/>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
       <c r="L18" s="54"/>
       <c r="M18" s="54"/>
       <c r="N18" s="54"/>
       <c r="O18" s="54"/>
-      <c r="P18" s="384"/>
-      <c r="Q18" s="384"/>
+      <c r="P18" s="171"/>
+      <c r="Q18" s="171"/>
       <c r="R18" s="109"/>
       <c r="S18" s="54"/>
       <c r="T18" s="54"/>
@@ -6998,15 +6998,15 @@
       <c r="B19" s="51"/>
       <c r="C19" s="52"/>
       <c r="D19" s="53"/>
-      <c r="E19" s="412">
+      <c r="E19" s="180">
         <v>13</v>
       </c>
-      <c r="F19" s="403" t="s">
+      <c r="F19" s="345" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="404"/>
-      <c r="H19" s="405"/>
-      <c r="I19" s="414"/>
+      <c r="G19" s="346"/>
+      <c r="H19" s="347"/>
+      <c r="I19" s="182"/>
       <c r="J19" s="54"/>
       <c r="K19" s="54"/>
       <c r="L19" s="54"/>
@@ -7037,15 +7037,15 @@
       <c r="B20" s="51"/>
       <c r="C20" s="52"/>
       <c r="D20" s="53"/>
-      <c r="E20" s="412">
+      <c r="E20" s="180">
         <v>14</v>
       </c>
-      <c r="F20" s="403" t="s">
+      <c r="F20" s="345" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="404"/>
-      <c r="H20" s="405"/>
-      <c r="I20" s="414"/>
+      <c r="G20" s="346"/>
+      <c r="H20" s="347"/>
+      <c r="I20" s="182"/>
       <c r="J20" s="54"/>
       <c r="K20" s="54"/>
       <c r="L20" s="54"/>
@@ -7076,15 +7076,15 @@
       <c r="B21" s="51"/>
       <c r="C21" s="52"/>
       <c r="D21" s="53"/>
-      <c r="E21" s="412">
+      <c r="E21" s="180">
         <v>15</v>
       </c>
-      <c r="F21" s="409" t="s">
+      <c r="F21" s="177" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="410"/>
-      <c r="H21" s="411"/>
-      <c r="I21" s="414"/>
+      <c r="G21" s="178"/>
+      <c r="H21" s="179"/>
+      <c r="I21" s="182"/>
       <c r="J21" s="54"/>
       <c r="K21" s="54"/>
       <c r="L21" s="54"/>
@@ -7157,9 +7157,9 @@
       <c r="E23" s="65">
         <v>1</v>
       </c>
-      <c r="F23" s="379"/>
-      <c r="G23" s="380"/>
-      <c r="H23" s="381"/>
+      <c r="F23" s="352"/>
+      <c r="G23" s="353"/>
+      <c r="H23" s="354"/>
       <c r="I23" s="66"/>
       <c r="J23" s="67"/>
       <c r="K23" s="67"/>
@@ -7194,9 +7194,9 @@
       <c r="E24" s="72">
         <v>2</v>
       </c>
-      <c r="F24" s="325"/>
-      <c r="G24" s="326"/>
-      <c r="H24" s="327"/>
+      <c r="F24" s="340"/>
+      <c r="G24" s="341"/>
+      <c r="H24" s="342"/>
       <c r="I24" s="73"/>
       <c r="J24" s="74"/>
       <c r="K24" s="74"/>
@@ -7231,9 +7231,9 @@
       <c r="E25" s="72">
         <v>3</v>
       </c>
-      <c r="F25" s="325"/>
-      <c r="G25" s="326"/>
-      <c r="H25" s="327"/>
+      <c r="F25" s="340"/>
+      <c r="G25" s="341"/>
+      <c r="H25" s="342"/>
       <c r="I25" s="73"/>
       <c r="J25" s="74"/>
       <c r="K25" s="74"/>
@@ -7268,9 +7268,9 @@
       <c r="E26" s="72">
         <v>4</v>
       </c>
-      <c r="F26" s="325"/>
-      <c r="G26" s="326"/>
-      <c r="H26" s="327"/>
+      <c r="F26" s="340"/>
+      <c r="G26" s="341"/>
+      <c r="H26" s="342"/>
       <c r="I26" s="73"/>
       <c r="J26" s="74"/>
       <c r="K26" s="74"/>
@@ -7305,9 +7305,9 @@
       <c r="E27" s="72">
         <v>5</v>
       </c>
-      <c r="F27" s="325"/>
-      <c r="G27" s="326"/>
-      <c r="H27" s="327"/>
+      <c r="F27" s="340"/>
+      <c r="G27" s="341"/>
+      <c r="H27" s="342"/>
       <c r="I27" s="73"/>
       <c r="J27" s="74"/>
       <c r="K27" s="74"/>
@@ -7336,33 +7336,33 @@
       <c r="AI27" s="50"/>
     </row>
     <row r="28" spans="2:35" s="39" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="328" t="s">
+      <c r="B28" s="386" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="329"/>
-      <c r="D28" s="329"/>
+      <c r="C28" s="387"/>
+      <c r="D28" s="387"/>
       <c r="E28" s="77"/>
       <c r="F28" s="78"/>
       <c r="G28" s="79"/>
       <c r="H28" s="80"/>
-      <c r="I28" s="345" t="s">
+      <c r="I28" s="390" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="345"/>
-      <c r="K28" s="345"/>
-      <c r="L28" s="345"/>
-      <c r="M28" s="345"/>
-      <c r="N28" s="345"/>
-      <c r="O28" s="345"/>
-      <c r="P28" s="345"/>
-      <c r="Q28" s="345"/>
-      <c r="R28" s="345"/>
-      <c r="S28" s="345"/>
-      <c r="T28" s="345"/>
-      <c r="U28" s="345"/>
-      <c r="V28" s="345"/>
-      <c r="W28" s="345"/>
-      <c r="X28" s="346"/>
+      <c r="J28" s="390"/>
+      <c r="K28" s="390"/>
+      <c r="L28" s="390"/>
+      <c r="M28" s="390"/>
+      <c r="N28" s="390"/>
+      <c r="O28" s="390"/>
+      <c r="P28" s="390"/>
+      <c r="Q28" s="390"/>
+      <c r="R28" s="390"/>
+      <c r="S28" s="390"/>
+      <c r="T28" s="390"/>
+      <c r="U28" s="390"/>
+      <c r="V28" s="390"/>
+      <c r="W28" s="390"/>
+      <c r="X28" s="391"/>
       <c r="Y28" s="81"/>
       <c r="Z28" s="82"/>
       <c r="AA28" s="82"/>
@@ -7375,15 +7375,15 @@
       <c r="AI28" s="50"/>
     </row>
     <row r="29" spans="2:35" s="39" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="347"/>
-      <c r="C29" s="350"/>
-      <c r="D29" s="353"/>
-      <c r="E29" s="356" t="s">
+      <c r="B29" s="392"/>
+      <c r="C29" s="395"/>
+      <c r="D29" s="398"/>
+      <c r="E29" s="401" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="356"/>
-      <c r="G29" s="356"/>
-      <c r="H29" s="357"/>
+      <c r="F29" s="401"/>
+      <c r="G29" s="401"/>
+      <c r="H29" s="402"/>
       <c r="I29" s="139"/>
       <c r="J29" s="85"/>
       <c r="K29" s="85"/>
@@ -7413,425 +7413,425 @@
       <c r="AI29" s="50"/>
     </row>
     <row r="30" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="348"/>
-      <c r="C30" s="351"/>
-      <c r="D30" s="354"/>
-      <c r="E30" s="356"/>
-      <c r="F30" s="356"/>
-      <c r="G30" s="356"/>
-      <c r="H30" s="357"/>
-      <c r="I30" s="387" t="s">
+      <c r="B30" s="393"/>
+      <c r="C30" s="396"/>
+      <c r="D30" s="399"/>
+      <c r="E30" s="401"/>
+      <c r="F30" s="401"/>
+      <c r="G30" s="401"/>
+      <c r="H30" s="402"/>
+      <c r="I30" s="403" t="s">
         <v>106</v>
       </c>
-      <c r="J30" s="388" t="s">
+      <c r="J30" s="337" t="s">
         <v>107</v>
       </c>
-      <c r="K30" s="388" t="s">
+      <c r="K30" s="337" t="s">
         <v>108</v>
       </c>
-      <c r="L30" s="388" t="s">
+      <c r="L30" s="337" t="s">
         <v>109</v>
       </c>
-      <c r="M30" s="388">
+      <c r="M30" s="337">
         <v>45476</v>
       </c>
-      <c r="N30" s="388" t="s">
+      <c r="N30" s="337" t="s">
         <v>110</v>
       </c>
-      <c r="O30" s="388" t="s">
+      <c r="O30" s="337" t="s">
         <v>111</v>
       </c>
-      <c r="P30" s="388" t="s">
+      <c r="P30" s="337" t="s">
         <v>112</v>
       </c>
-      <c r="Q30" s="388">
+      <c r="Q30" s="337">
         <v>45386</v>
       </c>
-      <c r="R30" s="388">
+      <c r="R30" s="337">
         <v>45600</v>
       </c>
-      <c r="S30" s="388" t="s">
+      <c r="S30" s="337" t="s">
         <v>113</v>
       </c>
-      <c r="T30" s="388" t="s">
+      <c r="T30" s="337" t="s">
         <v>114</v>
       </c>
-      <c r="U30" s="388" t="s">
+      <c r="U30" s="337" t="s">
         <v>113</v>
       </c>
-      <c r="V30" s="388" t="s">
+      <c r="V30" s="337" t="s">
         <v>114</v>
       </c>
-      <c r="W30" s="388"/>
-      <c r="X30" s="389">
+      <c r="W30" s="337"/>
+      <c r="X30" s="411">
         <v>45327</v>
       </c>
-      <c r="Y30" s="393" t="s">
+      <c r="Y30" s="370" t="s">
         <v>115</v>
       </c>
-      <c r="Z30" s="394" t="s">
+      <c r="Z30" s="368" t="s">
         <v>116</v>
       </c>
-      <c r="AA30" s="394" t="s">
+      <c r="AA30" s="368" t="s">
         <v>117</v>
       </c>
-      <c r="AB30" s="394" t="s">
+      <c r="AB30" s="368" t="s">
         <v>118</v>
       </c>
-      <c r="AC30" s="394" t="s">
+      <c r="AC30" s="368" t="s">
         <v>119</v>
       </c>
-      <c r="AD30" s="394" t="s">
+      <c r="AD30" s="368" t="s">
         <v>120</v>
       </c>
-      <c r="AE30" s="395" t="s">
+      <c r="AE30" s="413" t="s">
         <v>121</v>
       </c>
-      <c r="AG30" s="338"/>
+      <c r="AG30" s="410"/>
       <c r="AH30" s="50"/>
       <c r="AI30" s="50"/>
     </row>
     <row r="31" spans="2:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="348"/>
-      <c r="C31" s="351"/>
-      <c r="D31" s="354"/>
-      <c r="E31" s="356"/>
-      <c r="F31" s="356"/>
-      <c r="G31" s="356"/>
-      <c r="H31" s="357"/>
-      <c r="I31" s="387"/>
-      <c r="J31" s="388"/>
-      <c r="K31" s="388"/>
-      <c r="L31" s="388"/>
-      <c r="M31" s="388"/>
-      <c r="N31" s="388"/>
-      <c r="O31" s="388"/>
-      <c r="P31" s="388"/>
-      <c r="Q31" s="388"/>
-      <c r="R31" s="388"/>
-      <c r="S31" s="388"/>
-      <c r="T31" s="388"/>
-      <c r="U31" s="388"/>
-      <c r="V31" s="388"/>
-      <c r="W31" s="388"/>
-      <c r="X31" s="389"/>
-      <c r="Y31" s="396"/>
-      <c r="Z31" s="394"/>
-      <c r="AA31" s="394"/>
-      <c r="AB31" s="394"/>
-      <c r="AC31" s="394"/>
-      <c r="AD31" s="394"/>
-      <c r="AE31" s="395"/>
-      <c r="AG31" s="338"/>
+      <c r="B31" s="393"/>
+      <c r="C31" s="396"/>
+      <c r="D31" s="399"/>
+      <c r="E31" s="401"/>
+      <c r="F31" s="401"/>
+      <c r="G31" s="401"/>
+      <c r="H31" s="402"/>
+      <c r="I31" s="403"/>
+      <c r="J31" s="337"/>
+      <c r="K31" s="337"/>
+      <c r="L31" s="337"/>
+      <c r="M31" s="337"/>
+      <c r="N31" s="337"/>
+      <c r="O31" s="337"/>
+      <c r="P31" s="337"/>
+      <c r="Q31" s="337"/>
+      <c r="R31" s="337"/>
+      <c r="S31" s="337"/>
+      <c r="T31" s="337"/>
+      <c r="U31" s="337"/>
+      <c r="V31" s="337"/>
+      <c r="W31" s="337"/>
+      <c r="X31" s="411"/>
+      <c r="Y31" s="371"/>
+      <c r="Z31" s="368"/>
+      <c r="AA31" s="368"/>
+      <c r="AB31" s="368"/>
+      <c r="AC31" s="368"/>
+      <c r="AD31" s="368"/>
+      <c r="AE31" s="413"/>
+      <c r="AG31" s="410"/>
       <c r="AH31" s="50"/>
       <c r="AI31" s="50"/>
     </row>
     <row r="32" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="348"/>
-      <c r="C32" s="351"/>
-      <c r="D32" s="354"/>
-      <c r="E32" s="339" t="s">
+      <c r="B32" s="393"/>
+      <c r="C32" s="396"/>
+      <c r="D32" s="399"/>
+      <c r="E32" s="377" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="339"/>
-      <c r="G32" s="339"/>
-      <c r="H32" s="340"/>
-      <c r="I32" s="387"/>
-      <c r="J32" s="388"/>
-      <c r="K32" s="388"/>
-      <c r="L32" s="388"/>
-      <c r="M32" s="388"/>
-      <c r="N32" s="388"/>
-      <c r="O32" s="388"/>
-      <c r="P32" s="388"/>
-      <c r="Q32" s="388"/>
-      <c r="R32" s="388"/>
-      <c r="S32" s="388"/>
-      <c r="T32" s="388"/>
-      <c r="U32" s="388"/>
-      <c r="V32" s="388"/>
-      <c r="W32" s="388"/>
-      <c r="X32" s="389"/>
-      <c r="Y32" s="396"/>
-      <c r="Z32" s="394"/>
-      <c r="AA32" s="394"/>
-      <c r="AB32" s="394"/>
-      <c r="AC32" s="394"/>
-      <c r="AD32" s="394"/>
-      <c r="AE32" s="395"/>
-      <c r="AG32" s="338"/>
+      <c r="F32" s="377"/>
+      <c r="G32" s="377"/>
+      <c r="H32" s="378"/>
+      <c r="I32" s="403"/>
+      <c r="J32" s="337"/>
+      <c r="K32" s="337"/>
+      <c r="L32" s="337"/>
+      <c r="M32" s="337"/>
+      <c r="N32" s="337"/>
+      <c r="O32" s="337"/>
+      <c r="P32" s="337"/>
+      <c r="Q32" s="337"/>
+      <c r="R32" s="337"/>
+      <c r="S32" s="337"/>
+      <c r="T32" s="337"/>
+      <c r="U32" s="337"/>
+      <c r="V32" s="337"/>
+      <c r="W32" s="337"/>
+      <c r="X32" s="411"/>
+      <c r="Y32" s="371"/>
+      <c r="Z32" s="368"/>
+      <c r="AA32" s="368"/>
+      <c r="AB32" s="368"/>
+      <c r="AC32" s="368"/>
+      <c r="AD32" s="368"/>
+      <c r="AE32" s="413"/>
+      <c r="AG32" s="410"/>
       <c r="AH32" s="50"/>
       <c r="AI32" s="50"/>
     </row>
     <row r="33" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="348"/>
-      <c r="C33" s="351"/>
-      <c r="D33" s="354"/>
-      <c r="E33" s="331">
+      <c r="B33" s="393"/>
+      <c r="C33" s="396"/>
+      <c r="D33" s="399"/>
+      <c r="E33" s="364">
         <v>1</v>
       </c>
-      <c r="F33" s="332"/>
-      <c r="G33" s="332"/>
-      <c r="H33" s="333"/>
-      <c r="I33" s="387"/>
-      <c r="J33" s="388"/>
-      <c r="K33" s="388"/>
-      <c r="L33" s="388"/>
-      <c r="M33" s="388"/>
-      <c r="N33" s="388"/>
-      <c r="O33" s="388"/>
-      <c r="P33" s="388"/>
-      <c r="Q33" s="388"/>
-      <c r="R33" s="388"/>
-      <c r="S33" s="388"/>
-      <c r="T33" s="388"/>
-      <c r="U33" s="388"/>
-      <c r="V33" s="388"/>
-      <c r="W33" s="388"/>
-      <c r="X33" s="389"/>
-      <c r="Y33" s="396"/>
-      <c r="Z33" s="394"/>
-      <c r="AA33" s="394"/>
-      <c r="AB33" s="394"/>
-      <c r="AC33" s="394"/>
-      <c r="AD33" s="394"/>
-      <c r="AE33" s="395"/>
-      <c r="AG33" s="338"/>
+      <c r="F33" s="365"/>
+      <c r="G33" s="365"/>
+      <c r="H33" s="366"/>
+      <c r="I33" s="403"/>
+      <c r="J33" s="337"/>
+      <c r="K33" s="337"/>
+      <c r="L33" s="337"/>
+      <c r="M33" s="337"/>
+      <c r="N33" s="337"/>
+      <c r="O33" s="337"/>
+      <c r="P33" s="337"/>
+      <c r="Q33" s="337"/>
+      <c r="R33" s="337"/>
+      <c r="S33" s="337"/>
+      <c r="T33" s="337"/>
+      <c r="U33" s="337"/>
+      <c r="V33" s="337"/>
+      <c r="W33" s="337"/>
+      <c r="X33" s="411"/>
+      <c r="Y33" s="371"/>
+      <c r="Z33" s="368"/>
+      <c r="AA33" s="368"/>
+      <c r="AB33" s="368"/>
+      <c r="AC33" s="368"/>
+      <c r="AD33" s="368"/>
+      <c r="AE33" s="413"/>
+      <c r="AG33" s="410"/>
       <c r="AH33" s="50"/>
       <c r="AI33" s="50"/>
     </row>
     <row r="34" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="348"/>
-      <c r="C34" s="351"/>
-      <c r="D34" s="354"/>
-      <c r="E34" s="331">
+      <c r="B34" s="393"/>
+      <c r="C34" s="396"/>
+      <c r="D34" s="399"/>
+      <c r="E34" s="364">
         <v>2</v>
       </c>
-      <c r="F34" s="332"/>
-      <c r="G34" s="332"/>
-      <c r="H34" s="333"/>
-      <c r="I34" s="387"/>
-      <c r="J34" s="388"/>
-      <c r="K34" s="388"/>
-      <c r="L34" s="388"/>
-      <c r="M34" s="388"/>
-      <c r="N34" s="388"/>
-      <c r="O34" s="388"/>
-      <c r="P34" s="388"/>
-      <c r="Q34" s="388"/>
-      <c r="R34" s="388"/>
-      <c r="S34" s="388"/>
-      <c r="T34" s="388"/>
-      <c r="U34" s="388"/>
-      <c r="V34" s="388"/>
-      <c r="W34" s="388"/>
-      <c r="X34" s="389"/>
-      <c r="Y34" s="396"/>
-      <c r="Z34" s="394"/>
-      <c r="AA34" s="394"/>
-      <c r="AB34" s="394"/>
-      <c r="AC34" s="394"/>
-      <c r="AD34" s="394"/>
-      <c r="AE34" s="395"/>
-      <c r="AG34" s="338"/>
+      <c r="F34" s="365"/>
+      <c r="G34" s="365"/>
+      <c r="H34" s="366"/>
+      <c r="I34" s="403"/>
+      <c r="J34" s="337"/>
+      <c r="K34" s="337"/>
+      <c r="L34" s="337"/>
+      <c r="M34" s="337"/>
+      <c r="N34" s="337"/>
+      <c r="O34" s="337"/>
+      <c r="P34" s="337"/>
+      <c r="Q34" s="337"/>
+      <c r="R34" s="337"/>
+      <c r="S34" s="337"/>
+      <c r="T34" s="337"/>
+      <c r="U34" s="337"/>
+      <c r="V34" s="337"/>
+      <c r="W34" s="337"/>
+      <c r="X34" s="411"/>
+      <c r="Y34" s="371"/>
+      <c r="Z34" s="368"/>
+      <c r="AA34" s="368"/>
+      <c r="AB34" s="368"/>
+      <c r="AC34" s="368"/>
+      <c r="AD34" s="368"/>
+      <c r="AE34" s="413"/>
+      <c r="AG34" s="410"/>
       <c r="AH34" s="50"/>
       <c r="AI34" s="50"/>
     </row>
     <row r="35" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="348"/>
-      <c r="C35" s="351"/>
-      <c r="D35" s="354"/>
-      <c r="E35" s="331">
+      <c r="B35" s="393"/>
+      <c r="C35" s="396"/>
+      <c r="D35" s="399"/>
+      <c r="E35" s="364">
         <v>3</v>
       </c>
-      <c r="F35" s="332"/>
-      <c r="G35" s="332"/>
-      <c r="H35" s="333"/>
-      <c r="I35" s="387"/>
-      <c r="J35" s="388"/>
-      <c r="K35" s="388"/>
-      <c r="L35" s="388"/>
-      <c r="M35" s="388"/>
-      <c r="N35" s="388"/>
-      <c r="O35" s="388"/>
-      <c r="P35" s="388"/>
-      <c r="Q35" s="388"/>
-      <c r="R35" s="388"/>
-      <c r="S35" s="388"/>
-      <c r="T35" s="388"/>
-      <c r="U35" s="388"/>
-      <c r="V35" s="388"/>
-      <c r="W35" s="388"/>
-      <c r="X35" s="389"/>
-      <c r="Y35" s="396"/>
-      <c r="Z35" s="394"/>
-      <c r="AA35" s="394"/>
-      <c r="AB35" s="394"/>
-      <c r="AC35" s="394"/>
-      <c r="AD35" s="394"/>
-      <c r="AE35" s="395"/>
-      <c r="AG35" s="338"/>
+      <c r="F35" s="365"/>
+      <c r="G35" s="365"/>
+      <c r="H35" s="366"/>
+      <c r="I35" s="403"/>
+      <c r="J35" s="337"/>
+      <c r="K35" s="337"/>
+      <c r="L35" s="337"/>
+      <c r="M35" s="337"/>
+      <c r="N35" s="337"/>
+      <c r="O35" s="337"/>
+      <c r="P35" s="337"/>
+      <c r="Q35" s="337"/>
+      <c r="R35" s="337"/>
+      <c r="S35" s="337"/>
+      <c r="T35" s="337"/>
+      <c r="U35" s="337"/>
+      <c r="V35" s="337"/>
+      <c r="W35" s="337"/>
+      <c r="X35" s="411"/>
+      <c r="Y35" s="371"/>
+      <c r="Z35" s="368"/>
+      <c r="AA35" s="368"/>
+      <c r="AB35" s="368"/>
+      <c r="AC35" s="368"/>
+      <c r="AD35" s="368"/>
+      <c r="AE35" s="413"/>
+      <c r="AG35" s="410"/>
       <c r="AH35" s="50"/>
       <c r="AI35" s="50"/>
     </row>
     <row r="36" spans="2:35" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="348"/>
-      <c r="C36" s="351"/>
-      <c r="D36" s="354"/>
+      <c r="B36" s="393"/>
+      <c r="C36" s="396"/>
+      <c r="D36" s="399"/>
       <c r="E36" s="140" t="s">
         <v>60</v>
       </c>
       <c r="F36" s="129"/>
       <c r="G36" s="130"/>
       <c r="H36" s="131"/>
-      <c r="I36" s="390"/>
-      <c r="J36" s="391"/>
-      <c r="K36" s="391"/>
-      <c r="L36" s="391"/>
-      <c r="M36" s="391"/>
-      <c r="N36" s="391"/>
-      <c r="O36" s="391"/>
-      <c r="P36" s="391"/>
-      <c r="Q36" s="391"/>
-      <c r="R36" s="391"/>
-      <c r="S36" s="391"/>
-      <c r="T36" s="391"/>
-      <c r="U36" s="391"/>
-      <c r="V36" s="391"/>
-      <c r="W36" s="391"/>
-      <c r="X36" s="392"/>
-      <c r="Y36" s="397"/>
-      <c r="Z36" s="398"/>
-      <c r="AA36" s="398"/>
-      <c r="AB36" s="398"/>
-      <c r="AC36" s="398"/>
-      <c r="AD36" s="398"/>
-      <c r="AE36" s="399"/>
-      <c r="AG36" s="338"/>
+      <c r="I36" s="404"/>
+      <c r="J36" s="338"/>
+      <c r="K36" s="338"/>
+      <c r="L36" s="338"/>
+      <c r="M36" s="338"/>
+      <c r="N36" s="338"/>
+      <c r="O36" s="338"/>
+      <c r="P36" s="338"/>
+      <c r="Q36" s="338"/>
+      <c r="R36" s="338"/>
+      <c r="S36" s="338"/>
+      <c r="T36" s="338"/>
+      <c r="U36" s="338"/>
+      <c r="V36" s="338"/>
+      <c r="W36" s="338"/>
+      <c r="X36" s="412"/>
+      <c r="Y36" s="372"/>
+      <c r="Z36" s="369"/>
+      <c r="AA36" s="369"/>
+      <c r="AB36" s="369"/>
+      <c r="AC36" s="369"/>
+      <c r="AD36" s="369"/>
+      <c r="AE36" s="414"/>
+      <c r="AG36" s="410"/>
       <c r="AH36" s="23"/>
       <c r="AI36" s="23"/>
     </row>
     <row r="37" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="348"/>
-      <c r="C37" s="351"/>
-      <c r="D37" s="354"/>
-      <c r="E37" s="331">
+      <c r="B37" s="393"/>
+      <c r="C37" s="396"/>
+      <c r="D37" s="399"/>
+      <c r="E37" s="364">
         <v>1</v>
       </c>
-      <c r="F37" s="332"/>
-      <c r="G37" s="332"/>
-      <c r="H37" s="333"/>
-      <c r="I37" s="336" t="s">
+      <c r="F37" s="365"/>
+      <c r="G37" s="365"/>
+      <c r="H37" s="366"/>
+      <c r="I37" s="408" t="s">
         <v>61</v>
       </c>
-      <c r="J37" s="336"/>
-      <c r="K37" s="336"/>
-      <c r="L37" s="336"/>
-      <c r="M37" s="336"/>
-      <c r="N37" s="336"/>
-      <c r="O37" s="336"/>
-      <c r="P37" s="336"/>
-      <c r="Q37" s="336"/>
-      <c r="R37" s="336"/>
-      <c r="S37" s="336"/>
-      <c r="T37" s="336"/>
-      <c r="U37" s="336"/>
-      <c r="V37" s="336"/>
-      <c r="W37" s="336"/>
-      <c r="X37" s="336"/>
-      <c r="Y37" s="336"/>
-      <c r="Z37" s="336"/>
-      <c r="AA37" s="336"/>
-      <c r="AB37" s="336"/>
-      <c r="AC37" s="336"/>
-      <c r="AD37" s="336"/>
-      <c r="AE37" s="337"/>
-      <c r="AG37" s="338"/>
-      <c r="AH37" s="330"/>
-      <c r="AI37" s="330"/>
+      <c r="J37" s="408"/>
+      <c r="K37" s="408"/>
+      <c r="L37" s="408"/>
+      <c r="M37" s="408"/>
+      <c r="N37" s="408"/>
+      <c r="O37" s="408"/>
+      <c r="P37" s="408"/>
+      <c r="Q37" s="408"/>
+      <c r="R37" s="408"/>
+      <c r="S37" s="408"/>
+      <c r="T37" s="408"/>
+      <c r="U37" s="408"/>
+      <c r="V37" s="408"/>
+      <c r="W37" s="408"/>
+      <c r="X37" s="408"/>
+      <c r="Y37" s="408"/>
+      <c r="Z37" s="408"/>
+      <c r="AA37" s="408"/>
+      <c r="AB37" s="408"/>
+      <c r="AC37" s="408"/>
+      <c r="AD37" s="408"/>
+      <c r="AE37" s="409"/>
+      <c r="AG37" s="410"/>
+      <c r="AH37" s="405"/>
+      <c r="AI37" s="405"/>
     </row>
     <row r="38" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="348"/>
-      <c r="C38" s="351"/>
-      <c r="D38" s="354"/>
-      <c r="E38" s="331">
+      <c r="B38" s="393"/>
+      <c r="C38" s="396"/>
+      <c r="D38" s="399"/>
+      <c r="E38" s="364">
         <v>2</v>
       </c>
-      <c r="F38" s="332"/>
-      <c r="G38" s="332"/>
-      <c r="H38" s="333"/>
-      <c r="I38" s="336"/>
-      <c r="J38" s="336"/>
-      <c r="K38" s="336"/>
-      <c r="L38" s="336"/>
-      <c r="M38" s="336"/>
-      <c r="N38" s="336"/>
-      <c r="O38" s="336"/>
-      <c r="P38" s="336"/>
-      <c r="Q38" s="336"/>
-      <c r="R38" s="336"/>
-      <c r="S38" s="336"/>
-      <c r="T38" s="336"/>
-      <c r="U38" s="336"/>
-      <c r="V38" s="336"/>
-      <c r="W38" s="336"/>
-      <c r="X38" s="336"/>
-      <c r="Y38" s="336"/>
-      <c r="Z38" s="336"/>
-      <c r="AA38" s="336"/>
-      <c r="AB38" s="336"/>
-      <c r="AC38" s="336"/>
-      <c r="AD38" s="336"/>
-      <c r="AE38" s="337"/>
-      <c r="AG38" s="338"/>
+      <c r="F38" s="365"/>
+      <c r="G38" s="365"/>
+      <c r="H38" s="366"/>
+      <c r="I38" s="408"/>
+      <c r="J38" s="408"/>
+      <c r="K38" s="408"/>
+      <c r="L38" s="408"/>
+      <c r="M38" s="408"/>
+      <c r="N38" s="408"/>
+      <c r="O38" s="408"/>
+      <c r="P38" s="408"/>
+      <c r="Q38" s="408"/>
+      <c r="R38" s="408"/>
+      <c r="S38" s="408"/>
+      <c r="T38" s="408"/>
+      <c r="U38" s="408"/>
+      <c r="V38" s="408"/>
+      <c r="W38" s="408"/>
+      <c r="X38" s="408"/>
+      <c r="Y38" s="408"/>
+      <c r="Z38" s="408"/>
+      <c r="AA38" s="408"/>
+      <c r="AB38" s="408"/>
+      <c r="AC38" s="408"/>
+      <c r="AD38" s="408"/>
+      <c r="AE38" s="409"/>
+      <c r="AG38" s="410"/>
     </row>
     <row r="39" spans="2:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="348"/>
-      <c r="C39" s="351"/>
-      <c r="D39" s="354"/>
-      <c r="E39" s="331">
+      <c r="B39" s="393"/>
+      <c r="C39" s="396"/>
+      <c r="D39" s="399"/>
+      <c r="E39" s="364">
         <v>3</v>
       </c>
-      <c r="F39" s="332"/>
-      <c r="G39" s="332"/>
-      <c r="H39" s="333"/>
-      <c r="I39" s="334"/>
-      <c r="J39" s="335"/>
-      <c r="K39" s="335"/>
-      <c r="L39" s="335"/>
-      <c r="M39" s="335"/>
-      <c r="N39" s="335"/>
-      <c r="O39" s="335"/>
-      <c r="P39" s="335"/>
-      <c r="Q39" s="335"/>
-      <c r="R39" s="335"/>
-      <c r="S39" s="335"/>
-      <c r="T39" s="335"/>
-      <c r="U39" s="335"/>
-      <c r="V39" s="335"/>
-      <c r="W39" s="335"/>
-      <c r="X39" s="335"/>
-      <c r="Y39" s="335"/>
-      <c r="Z39" s="335"/>
-      <c r="AA39" s="335"/>
-      <c r="AB39" s="335"/>
-      <c r="AC39" s="335"/>
-      <c r="AD39" s="335"/>
+      <c r="F39" s="365"/>
+      <c r="G39" s="365"/>
+      <c r="H39" s="366"/>
+      <c r="I39" s="406"/>
+      <c r="J39" s="407"/>
+      <c r="K39" s="407"/>
+      <c r="L39" s="407"/>
+      <c r="M39" s="407"/>
+      <c r="N39" s="407"/>
+      <c r="O39" s="407"/>
+      <c r="P39" s="407"/>
+      <c r="Q39" s="407"/>
+      <c r="R39" s="407"/>
+      <c r="S39" s="407"/>
+      <c r="T39" s="407"/>
+      <c r="U39" s="407"/>
+      <c r="V39" s="407"/>
+      <c r="W39" s="407"/>
+      <c r="X39" s="407"/>
+      <c r="Y39" s="407"/>
+      <c r="Z39" s="407"/>
+      <c r="AA39" s="407"/>
+      <c r="AB39" s="407"/>
+      <c r="AC39" s="407"/>
+      <c r="AD39" s="407"/>
       <c r="AE39" s="141"/>
-      <c r="AG39" s="338"/>
+      <c r="AG39" s="410"/>
       <c r="AH39" s="87"/>
       <c r="AI39" s="88"/>
     </row>
     <row r="40" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="348"/>
-      <c r="C40" s="351"/>
-      <c r="D40" s="354"/>
-      <c r="E40" s="339" t="s">
+      <c r="B40" s="393"/>
+      <c r="C40" s="396"/>
+      <c r="D40" s="399"/>
+      <c r="E40" s="377" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="339"/>
-      <c r="G40" s="339"/>
-      <c r="H40" s="340"/>
+      <c r="F40" s="377"/>
+      <c r="G40" s="377"/>
+      <c r="H40" s="378"/>
       <c r="I40" s="142"/>
       <c r="J40" s="143"/>
       <c r="K40" s="143"/>
@@ -7855,20 +7855,20 @@
       <c r="AC40" s="143"/>
       <c r="AD40" s="143"/>
       <c r="AE40" s="141"/>
-      <c r="AG40" s="338"/>
+      <c r="AG40" s="410"/>
       <c r="AH40" s="87"/>
       <c r="AI40" s="89"/>
     </row>
     <row r="41" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="348"/>
-      <c r="C41" s="351"/>
-      <c r="D41" s="354"/>
-      <c r="E41" s="331">
+      <c r="B41" s="393"/>
+      <c r="C41" s="396"/>
+      <c r="D41" s="399"/>
+      <c r="E41" s="364">
         <v>1</v>
       </c>
-      <c r="F41" s="332"/>
-      <c r="G41" s="332"/>
-      <c r="H41" s="333"/>
+      <c r="F41" s="365"/>
+      <c r="G41" s="365"/>
+      <c r="H41" s="366"/>
       <c r="I41" s="142"/>
       <c r="J41" s="143"/>
       <c r="K41" s="143"/>
@@ -7892,20 +7892,20 @@
       <c r="AC41" s="143"/>
       <c r="AD41" s="143"/>
       <c r="AE41" s="141"/>
-      <c r="AG41" s="338"/>
+      <c r="AG41" s="410"/>
       <c r="AH41" s="87"/>
       <c r="AI41" s="88"/>
     </row>
     <row r="42" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="348"/>
-      <c r="C42" s="351"/>
-      <c r="D42" s="354"/>
-      <c r="E42" s="331">
+      <c r="B42" s="393"/>
+      <c r="C42" s="396"/>
+      <c r="D42" s="399"/>
+      <c r="E42" s="364">
         <v>2</v>
       </c>
-      <c r="F42" s="332"/>
-      <c r="G42" s="332"/>
-      <c r="H42" s="333"/>
+      <c r="F42" s="365"/>
+      <c r="G42" s="365"/>
+      <c r="H42" s="366"/>
       <c r="I42" s="142"/>
       <c r="J42" s="143"/>
       <c r="K42" s="143"/>
@@ -7929,20 +7929,20 @@
       <c r="AC42" s="143"/>
       <c r="AD42" s="143"/>
       <c r="AE42" s="141"/>
-      <c r="AG42" s="338"/>
+      <c r="AG42" s="410"/>
       <c r="AH42" s="87"/>
       <c r="AI42" s="88"/>
     </row>
     <row r="43" spans="2:35" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="348"/>
-      <c r="C43" s="351"/>
-      <c r="D43" s="354"/>
-      <c r="E43" s="359">
+      <c r="B43" s="393"/>
+      <c r="C43" s="396"/>
+      <c r="D43" s="399"/>
+      <c r="E43" s="379">
         <v>3</v>
       </c>
-      <c r="F43" s="360"/>
-      <c r="G43" s="360"/>
-      <c r="H43" s="361"/>
+      <c r="F43" s="380"/>
+      <c r="G43" s="380"/>
+      <c r="H43" s="381"/>
       <c r="I43" s="144"/>
       <c r="J43" s="145"/>
       <c r="K43" s="145"/>
@@ -7966,53 +7966,53 @@
       <c r="AC43" s="145"/>
       <c r="AD43" s="145"/>
       <c r="AE43" s="146"/>
-      <c r="AG43" s="338"/>
+      <c r="AG43" s="410"/>
       <c r="AH43" s="90"/>
       <c r="AI43" s="90"/>
     </row>
     <row r="44" spans="2:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="348"/>
-      <c r="C44" s="351"/>
-      <c r="D44" s="354"/>
-      <c r="E44" s="362" t="s">
+      <c r="B44" s="393"/>
+      <c r="C44" s="396"/>
+      <c r="D44" s="399"/>
+      <c r="E44" s="382" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="363"/>
-      <c r="G44" s="363"/>
-      <c r="H44" s="363"/>
-      <c r="I44" s="364"/>
-      <c r="J44" s="364"/>
-      <c r="K44" s="364"/>
-      <c r="L44" s="364"/>
-      <c r="M44" s="364"/>
-      <c r="N44" s="364"/>
-      <c r="O44" s="364"/>
-      <c r="P44" s="364"/>
-      <c r="Q44" s="364"/>
-      <c r="R44" s="364"/>
-      <c r="S44" s="364"/>
-      <c r="T44" s="364"/>
-      <c r="U44" s="364"/>
-      <c r="V44" s="364"/>
-      <c r="W44" s="364"/>
-      <c r="X44" s="364"/>
-      <c r="Y44" s="364"/>
-      <c r="Z44" s="364"/>
-      <c r="AA44" s="364"/>
-      <c r="AB44" s="364"/>
-      <c r="AC44" s="364"/>
-      <c r="AD44" s="364"/>
-      <c r="AE44" s="365"/>
-      <c r="AG44" s="338"/>
+      <c r="F44" s="383"/>
+      <c r="G44" s="383"/>
+      <c r="H44" s="383"/>
+      <c r="I44" s="384"/>
+      <c r="J44" s="384"/>
+      <c r="K44" s="384"/>
+      <c r="L44" s="384"/>
+      <c r="M44" s="384"/>
+      <c r="N44" s="384"/>
+      <c r="O44" s="384"/>
+      <c r="P44" s="384"/>
+      <c r="Q44" s="384"/>
+      <c r="R44" s="384"/>
+      <c r="S44" s="384"/>
+      <c r="T44" s="384"/>
+      <c r="U44" s="384"/>
+      <c r="V44" s="384"/>
+      <c r="W44" s="384"/>
+      <c r="X44" s="384"/>
+      <c r="Y44" s="384"/>
+      <c r="Z44" s="384"/>
+      <c r="AA44" s="384"/>
+      <c r="AB44" s="384"/>
+      <c r="AC44" s="384"/>
+      <c r="AD44" s="384"/>
+      <c r="AE44" s="385"/>
+      <c r="AG44" s="410"/>
     </row>
     <row r="45" spans="2:35" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="348"/>
-      <c r="C45" s="351"/>
-      <c r="D45" s="354"/>
-      <c r="E45" s="363" t="s">
+      <c r="B45" s="393"/>
+      <c r="C45" s="396"/>
+      <c r="D45" s="399"/>
+      <c r="E45" s="383" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="363"/>
+      <c r="F45" s="383"/>
       <c r="G45" s="91" t="s">
         <v>65</v>
       </c>
@@ -8044,16 +8044,16 @@
       <c r="AC45" s="93"/>
       <c r="AD45" s="91"/>
       <c r="AE45" s="94"/>
-      <c r="AG45" s="338"/>
+      <c r="AG45" s="410"/>
     </row>
     <row r="46" spans="2:35" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="348"/>
-      <c r="C46" s="351"/>
-      <c r="D46" s="354"/>
-      <c r="E46" s="371" t="s">
+      <c r="B46" s="393"/>
+      <c r="C46" s="396"/>
+      <c r="D46" s="399"/>
+      <c r="E46" s="367" t="s">
         <v>70</v>
       </c>
-      <c r="F46" s="371"/>
+      <c r="F46" s="367"/>
       <c r="G46" s="91" t="s">
         <v>71</v>
       </c>
@@ -8090,14 +8090,14 @@
       <c r="AC46" s="105"/>
       <c r="AD46" s="95"/>
       <c r="AE46" s="100"/>
-      <c r="AG46" s="338"/>
+      <c r="AG46" s="410"/>
     </row>
     <row r="47" spans="2:35" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="349"/>
-      <c r="C47" s="352"/>
-      <c r="D47" s="355"/>
-      <c r="E47" s="358"/>
-      <c r="F47" s="358"/>
+      <c r="B47" s="394"/>
+      <c r="C47" s="397"/>
+      <c r="D47" s="400"/>
+      <c r="E47" s="376"/>
+      <c r="F47" s="376"/>
       <c r="G47" s="101" t="s">
         <v>74</v>
       </c>
@@ -8125,7 +8125,7 @@
       <c r="AC47" s="101"/>
       <c r="AD47" s="101"/>
       <c r="AE47" s="102"/>
-      <c r="AG47" s="338"/>
+      <c r="AG47" s="410"/>
     </row>
     <row r="49" spans="10:35" x14ac:dyDescent="0.25">
       <c r="M49" s="92"/>
@@ -8197,26 +8197,45 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="P30:P36"/>
-    <mergeCell ref="Q30:Q36"/>
-    <mergeCell ref="K30:K36"/>
-    <mergeCell ref="L30:L36"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="G4:J5"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="AH37:AI37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="I39:X39"/>
+    <mergeCell ref="Y39:AA39"/>
+    <mergeCell ref="AB39:AD39"/>
+    <mergeCell ref="I37:AE38"/>
+    <mergeCell ref="AG30:AG47"/>
+    <mergeCell ref="U30:U36"/>
+    <mergeCell ref="V30:V36"/>
+    <mergeCell ref="W30:W36"/>
+    <mergeCell ref="X30:X36"/>
+    <mergeCell ref="AE30:AE36"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="I6:X6"/>
+    <mergeCell ref="AA30:AA36"/>
+    <mergeCell ref="AB30:AB36"/>
+    <mergeCell ref="AC30:AC36"/>
+    <mergeCell ref="I28:X28"/>
+    <mergeCell ref="B29:B47"/>
+    <mergeCell ref="C29:C47"/>
+    <mergeCell ref="D29:D47"/>
+    <mergeCell ref="E29:H31"/>
+    <mergeCell ref="I30:I36"/>
+    <mergeCell ref="J30:J36"/>
+    <mergeCell ref="O30:O36"/>
+    <mergeCell ref="R30:R36"/>
+    <mergeCell ref="S30:S36"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:AE44"/>
+    <mergeCell ref="E45:F45"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="Y6:AE6"/>
     <mergeCell ref="AB2:AE2"/>
@@ -8233,45 +8252,14 @@
     <mergeCell ref="E2:V2"/>
     <mergeCell ref="S3:AC3"/>
     <mergeCell ref="S4:AC4"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E44:AE44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="I6:X6"/>
-    <mergeCell ref="AA30:AA36"/>
-    <mergeCell ref="AB30:AB36"/>
-    <mergeCell ref="AC30:AC36"/>
-    <mergeCell ref="I28:X28"/>
-    <mergeCell ref="B29:B47"/>
-    <mergeCell ref="C29:C47"/>
-    <mergeCell ref="D29:D47"/>
-    <mergeCell ref="E29:H31"/>
-    <mergeCell ref="I30:I36"/>
-    <mergeCell ref="J30:J36"/>
-    <mergeCell ref="O30:O36"/>
-    <mergeCell ref="R30:R36"/>
-    <mergeCell ref="S30:S36"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="AH37:AI37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="I39:X39"/>
-    <mergeCell ref="Y39:AA39"/>
-    <mergeCell ref="AB39:AD39"/>
-    <mergeCell ref="I37:AE38"/>
-    <mergeCell ref="AG30:AG47"/>
-    <mergeCell ref="U30:U36"/>
-    <mergeCell ref="V30:V36"/>
-    <mergeCell ref="W30:W36"/>
-    <mergeCell ref="X30:X36"/>
-    <mergeCell ref="AE30:AE36"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="G4:J5"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F13:H13"/>
@@ -8279,6 +8267,18 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="P30:P36"/>
+    <mergeCell ref="Q30:Q36"/>
+    <mergeCell ref="K30:K36"/>
+    <mergeCell ref="L30:L36"/>
+    <mergeCell ref="N3:R3"/>
   </mergeCells>
   <conditionalFormatting sqref="H50:I50 U50 W50:AI50">
     <cfRule type="cellIs" dxfId="26" priority="25" stopIfTrue="1" operator="equal">
@@ -8392,7 +8392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7E2FC0-EC84-4725-8BB8-7200D21F2260}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>